<commit_message>
added gradient calculation to manual
</commit_message>
<xml_diff>
--- a/Combo/sampleTableaux.xlsx
+++ b/Combo/sampleTableaux.xlsx
@@ -1,103 +1,104 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clairemoore-cantwell/GitHub/GLaPL/Combo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clairemoore-cantwell/GitHub/GSR_Learning/Combo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC2E45D-D019-E94E-98CC-CF663347F133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB203C02-2D5B-BF4B-8F93-258FCCDB1172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28820" yWindow="460" windowWidth="38160" windowHeight="19320" activeTab="1" xr2:uid="{6D016418-8590-7F42-9768-866F63012115}"/>
+    <workbookView xWindow="7200" yWindow="2220" windowWidth="28800" windowHeight="17540" xr2:uid="{6D016418-8590-7F42-9768-866F63012115}"/>
   </bookViews>
   <sheets>
-    <sheet name="GSRTab" sheetId="1" r:id="rId1"/>
-    <sheet name="GSRTab_hidden" sheetId="6" r:id="rId2"/>
-    <sheet name="RSTTab" sheetId="2" r:id="rId3"/>
-    <sheet name="RSTTab_hidden" sheetId="3" r:id="rId4"/>
-    <sheet name="secretCalculator" sheetId="5" r:id="rId5"/>
+    <sheet name="LikelihoodCalcEx" sheetId="7" r:id="rId1"/>
+    <sheet name="GSRTab" sheetId="1" r:id="rId2"/>
+    <sheet name="GSRTab_hidden" sheetId="6" r:id="rId3"/>
+    <sheet name="RSTTab" sheetId="2" r:id="rId4"/>
+    <sheet name="RSTTab_hidden" sheetId="3" r:id="rId5"/>
+    <sheet name="secretCalculator" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">GSRTab!$E$5:$R$5</definedName>
-    <definedName name="solver_adj" localSheetId="2" hidden="1">RSTTab!$E$5:$R$5</definedName>
-    <definedName name="solver_adj" localSheetId="3" hidden="1">RSTTab_hidden!$F$6:$S$6</definedName>
-    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
-    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">GSRTab!$E$5:$R$5</definedName>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">RSTTab!$E$5:$R$5</definedName>
+    <definedName name="solver_adj" localSheetId="4" hidden="1">RSTTab_hidden!$F$6:$S$6</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_eng" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_lin" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_lin" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_lin" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_lin" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
-    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
+    <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
-    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
-    <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
+    <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
-    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_num" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_num" localSheetId="3" hidden="1">0</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">GSRTab!$X$9</definedName>
-    <definedName name="solver_opt" localSheetId="2" hidden="1">RSTTab!$X$8</definedName>
-    <definedName name="solver_opt" localSheetId="3" hidden="1">RSTTab_hidden!$Z$11</definedName>
-    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
-    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
+    <definedName name="solver_num" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">GSRTab!$X$9</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">RSTTab!$X$8</definedName>
+    <definedName name="solver_opt" localSheetId="4" hidden="1">RSTTab_hidden!$Z$11</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
-    <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
-    <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
-    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
+    <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
-    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
-    <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
+    <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_typ" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_ver" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_ver" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="4" hidden="1">2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -510,7 +511,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -532,7 +533,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="109">
   <si>
     <t>petit_ami</t>
   </si>
@@ -836,12 +837,36 @@
   <si>
     <t>sigmas:</t>
   </si>
+  <si>
+    <t>input_1</t>
+  </si>
+  <si>
+    <t>cand_1</t>
+  </si>
+  <si>
+    <t>input_2</t>
+  </si>
+  <si>
+    <t>cand_2</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>Observed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -863,12 +888,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1019,7 +1038,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1066,7 +1085,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1081,19 +1100,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1110,7 +1129,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1170,18 +1189,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1694,6 +1744,348 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0046436D-BC8C-DF40-9DB5-7AA4E3FA7FF9}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13" style="60" customWidth="1"/>
+    <col min="2" max="4" width="10.83203125" style="60"/>
+    <col min="5" max="5" width="9.33203125" style="61" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" style="62" customWidth="1"/>
+    <col min="7" max="7" width="1.1640625" style="62" customWidth="1"/>
+    <col min="8" max="8" width="7" style="62" customWidth="1"/>
+    <col min="9" max="10" width="9.6640625" style="63" customWidth="1"/>
+    <col min="11" max="11" width="10.1640625" style="62" customWidth="1"/>
+    <col min="12" max="12" width="13" style="60" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="60"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B2" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="61">
+        <f>(C5-C3)*SQRT(2)/$A$3^2</f>
+        <v>1.5556349186104048E-4</v>
+      </c>
+      <c r="D2" s="61">
+        <f>(D5-D3)*SQRT(2)/$A$3^2</f>
+        <v>3.2526911934581182E-4</v>
+      </c>
+      <c r="E2" s="61">
+        <f>(E5-E3)*SQRT(2)/$A$3^2</f>
+        <v>6.7882250993908557E-4</v>
+      </c>
+      <c r="H2" s="63"/>
+      <c r="I2" s="62">
+        <f>LN(1)</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="60">
+        <v>100</v>
+      </c>
+      <c r="B3" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="61">
+        <v>0</v>
+      </c>
+      <c r="D3" s="61">
+        <v>0</v>
+      </c>
+      <c r="E3" s="61">
+        <v>0</v>
+      </c>
+      <c r="H3" s="63"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B4" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="61">
+        <f>(C5-C3)^2/2/$A$3</f>
+        <v>6.0500000000000007E-3</v>
+      </c>
+      <c r="D4" s="61">
+        <f>(D5-D3)^2/2/$A$3</f>
+        <v>2.6449999999999994E-2</v>
+      </c>
+      <c r="E4" s="61">
+        <f>(E5-E3)^2/2/$A$3</f>
+        <v>0.1152</v>
+      </c>
+      <c r="H4" s="63"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+    </row>
+    <row r="5" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="61">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D5" s="61">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E5" s="61">
+        <v>4.8</v>
+      </c>
+      <c r="H5" s="63"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+    </row>
+    <row r="6" spans="1:11" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="64" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="65" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" s="65" t="s">
+        <v>107</v>
+      </c>
+      <c r="F6" s="66" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="67" t="s">
+        <v>99</v>
+      </c>
+      <c r="I6" s="66" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="64" t="e">
+        <f>SUMPRODUCT(J9)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K6" s="64" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="60" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" s="61">
+        <v>1</v>
+      </c>
+      <c r="D7" s="61">
+        <v>1</v>
+      </c>
+      <c r="E7" s="61">
+        <v>0</v>
+      </c>
+      <c r="F7" s="62">
+        <f>-SUMPRODUCT(C$5:E$5,C7:E7)</f>
+        <v>-3.4</v>
+      </c>
+      <c r="G7" s="62">
+        <f t="shared" ref="G7:G11" si="0">EXP(F7)</f>
+        <v>3.337326996032608E-2</v>
+      </c>
+      <c r="H7" s="63">
+        <f>G7/SUMIF(A:A,A7,G:G)</f>
+        <v>0.24472309568759198</v>
+      </c>
+      <c r="I7" s="62">
+        <f>LN(H7)</f>
+        <v>-1.4076279293028919</v>
+      </c>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="60" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="61">
+        <v>1</v>
+      </c>
+      <c r="D8" s="61">
+        <v>0</v>
+      </c>
+      <c r="E8" s="61">
+        <v>1</v>
+      </c>
+      <c r="F8" s="62">
+        <f>-SUMPRODUCT(C$5:E$5,C8:E8)</f>
+        <v>-5.9</v>
+      </c>
+      <c r="G8" s="62">
+        <f t="shared" si="0"/>
+        <v>2.7394448187683684E-3</v>
+      </c>
+      <c r="H8" s="63">
+        <f t="shared" ref="H8:H11" si="1">G8/SUMIF(A:A,A8,G:G)</f>
+        <v>2.0088094972752234E-2</v>
+      </c>
+      <c r="I8" s="62">
+        <f t="shared" ref="I8:I11" si="2">LN(H8)</f>
+        <v>-3.9076279293028922</v>
+      </c>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="60" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" s="61">
+        <v>0</v>
+      </c>
+      <c r="D9" s="61">
+        <v>1</v>
+      </c>
+      <c r="E9" s="61">
+        <v>0</v>
+      </c>
+      <c r="F9" s="62">
+        <f>-SUMPRODUCT(C$5:E$5,C9:E9)</f>
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="G9" s="62">
+        <f t="shared" si="0"/>
+        <v>0.10025884372280375</v>
+      </c>
+      <c r="H9" s="63">
+        <f t="shared" si="1"/>
+        <v>0.7351888093396558</v>
+      </c>
+      <c r="I9" s="62">
+        <f t="shared" si="2"/>
+        <v>-0.30762792930289173</v>
+      </c>
+      <c r="J9" s="60"/>
+      <c r="K9" s="60">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="68" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10" s="69">
+        <v>0</v>
+      </c>
+      <c r="D10" s="69">
+        <v>0</v>
+      </c>
+      <c r="E10" s="69">
+        <v>1</v>
+      </c>
+      <c r="F10" s="70">
+        <f>-SUMPRODUCT(C$5:E$5,C10:E10)</f>
+        <v>-4.8</v>
+      </c>
+      <c r="G10" s="70">
+        <f t="shared" si="0"/>
+        <v>8.2297470490200302E-3</v>
+      </c>
+      <c r="H10" s="71">
+        <f t="shared" si="1"/>
+        <v>2.4127021417669207E-2</v>
+      </c>
+      <c r="I10" s="70">
+        <f t="shared" si="2"/>
+        <v>-3.7244228459337791</v>
+      </c>
+      <c r="K10" s="68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" s="60" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" s="61">
+        <v>1</v>
+      </c>
+      <c r="D11" s="61">
+        <v>0</v>
+      </c>
+      <c r="E11" s="61">
+        <v>0</v>
+      </c>
+      <c r="F11" s="62">
+        <f>-SUMPRODUCT(C$5:E$5,C11:E11)</f>
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="G11" s="62">
+        <f t="shared" si="0"/>
+        <v>0.33287108369807955</v>
+      </c>
+      <c r="H11" s="63">
+        <f t="shared" si="1"/>
+        <v>0.9758729785823308</v>
+      </c>
+      <c r="I11" s="62">
+        <f t="shared" si="2"/>
+        <v>-2.442284593377916E-2</v>
+      </c>
+      <c r="J11" s="60"/>
+      <c r="K11" s="72">
+        <v>345</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{849952CB-BA06-6C44-855B-3B3D98D8050D}">
   <dimension ref="A2:X50"/>
   <sheetViews>
@@ -2054,15 +2446,15 @@
       <c r="Q7" s="10"/>
       <c r="R7" s="10"/>
       <c r="S7" s="24">
-        <f>-SUMPRODUCT(E$5:I$5,E7:I7)</f>
+        <f t="shared" ref="S7:S50" si="2">-SUMPRODUCT(E$5:I$5,E7:I7)</f>
         <v>5.3397163067732203</v>
       </c>
       <c r="T7" s="27">
-        <f t="shared" ref="T7:T50" si="2">EXP(S7)</f>
+        <f t="shared" ref="T7:T50" si="3">EXP(S7)</f>
         <v>208.45356503544042</v>
       </c>
       <c r="U7" s="48">
-        <f>T7/SUMIF(A:A,A7,T:T)</f>
+        <f t="shared" ref="U7:U50" si="4">T7/SUMIF(A:A,A7,T:T)</f>
         <v>0.92191403574481268</v>
       </c>
       <c r="V7" s="28">
@@ -2104,19 +2496,19 @@
       <c r="Q8" s="11"/>
       <c r="R8" s="11"/>
       <c r="S8" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E8:I8)</f>
+        <f t="shared" si="2"/>
         <v>2.8703309851518783</v>
       </c>
       <c r="T8" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17.642856757169465</v>
       </c>
       <c r="U8" s="46">
-        <f>T8/SUMIF(A:A,A8,T:T)</f>
+        <f t="shared" si="4"/>
         <v>7.8027916060367672E-2</v>
       </c>
       <c r="V8" s="29">
-        <f t="shared" ref="V8:V50" si="3">LN(U8)</f>
+        <f t="shared" ref="V8:V50" si="5">LN(U8)</f>
         <v>-2.5506886181129906</v>
       </c>
       <c r="W8" s="2" t="s">
@@ -2163,19 +2555,19 @@
       <c r="Q9" s="11"/>
       <c r="R9" s="11"/>
       <c r="S9" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E9:I9)</f>
+        <f t="shared" si="2"/>
         <v>-5.8003761906401374</v>
       </c>
       <c r="T9" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.0264160218201018E-3</v>
       </c>
       <c r="U9" s="46">
-        <f>T9/SUMIF(A:A,A9,T:T)</f>
+        <f t="shared" si="4"/>
         <v>1.3384733468312573E-5</v>
       </c>
       <c r="V9" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-11.221395793905007</v>
       </c>
       <c r="W9" s="2" t="s">
@@ -2222,19 +2614,19 @@
       <c r="Q10" s="11"/>
       <c r="R10" s="11"/>
       <c r="S10" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E10:I10)</f>
+        <f t="shared" si="2"/>
         <v>-5.8003764092237127</v>
       </c>
       <c r="T10" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.0264153602953398E-3</v>
       </c>
       <c r="U10" s="46">
-        <f>T10/SUMIF(A:A,A10,T:T)</f>
+        <f t="shared" si="4"/>
         <v>1.3384730542629997E-5</v>
       </c>
       <c r="V10" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-11.221396012488581</v>
       </c>
     </row>
@@ -2272,19 +2664,19 @@
       <c r="Q11" s="11"/>
       <c r="R11" s="11"/>
       <c r="S11" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E11:I11)</f>
+        <f t="shared" si="2"/>
         <v>-5</v>
       </c>
       <c r="T11" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.737946999085467E-3</v>
       </c>
       <c r="U11" s="46">
-        <f>T11/SUMIF(A:A,A11,T:T)</f>
+        <f t="shared" si="4"/>
         <v>2.979948032793503E-5</v>
       </c>
       <c r="V11" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-10.421019603264869</v>
       </c>
     </row>
@@ -2324,19 +2716,19 @@
       <c r="Q12" s="11"/>
       <c r="R12" s="11"/>
       <c r="S12" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E12:I12)</f>
+        <f t="shared" si="2"/>
         <v>-8.4634363322403772</v>
       </c>
       <c r="T12" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.1104560039106028E-4</v>
       </c>
       <c r="U12" s="46">
-        <f>T12/SUMIF(A:A,A12,T:T)</f>
+        <f t="shared" si="4"/>
         <v>9.3337766206891259E-7</v>
       </c>
       <c r="V12" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-13.884455935505246</v>
       </c>
     </row>
@@ -2376,19 +2768,19 @@
       <c r="Q13" s="11"/>
       <c r="R13" s="11"/>
       <c r="S13" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E13:I13)</f>
+        <f t="shared" si="2"/>
         <v>-9.6930072889179062</v>
       </c>
       <c r="T13" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.1713534647208962E-5</v>
       </c>
       <c r="U13" s="46">
-        <f>T13/SUMIF(A:A,A13,T:T)</f>
+        <f t="shared" si="4"/>
         <v>2.7293643923534123E-7</v>
       </c>
       <c r="V13" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-15.114026892182775</v>
       </c>
     </row>
@@ -2428,19 +2820,19 @@
       <c r="Q14" s="11"/>
       <c r="R14" s="11"/>
       <c r="S14" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E14:I14)</f>
+        <f t="shared" si="2"/>
         <v>-9.6930075075014823</v>
       </c>
       <c r="T14" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.1713521157645343E-5</v>
       </c>
       <c r="U14" s="46">
-        <f>T14/SUMIF(A:A,A14,T:T)</f>
+        <f t="shared" si="4"/>
         <v>2.7293637957592481E-7</v>
       </c>
       <c r="V14" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-15.114027110766351</v>
       </c>
     </row>
@@ -2484,19 +2876,19 @@
       <c r="Q15" s="10"/>
       <c r="R15" s="10"/>
       <c r="S15" s="24">
-        <f>-SUMPRODUCT(E$5:I$5,E15:I15)</f>
+        <f t="shared" si="2"/>
         <v>8.4135603715256426</v>
       </c>
       <c r="T15" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4507.7813509204989</v>
       </c>
       <c r="U15" s="48">
-        <f>T15/SUMIF(A:A,A15,T:T)</f>
+        <f t="shared" si="4"/>
         <v>0.99608238059463006</v>
       </c>
       <c r="V15" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-3.9253133775497776E-3</v>
       </c>
     </row>
@@ -2535,19 +2927,19 @@
       <c r="Q16" s="11"/>
       <c r="R16" s="11"/>
       <c r="S16" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E16:I16)</f>
+        <f t="shared" si="2"/>
         <v>2.8703309851518783</v>
       </c>
       <c r="T16" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17.642856757169465</v>
       </c>
       <c r="U16" s="46">
-        <f>T16/SUMIF(A:A,A16,T:T)</f>
+        <f t="shared" si="4"/>
         <v>3.8985339773817598E-3</v>
       </c>
       <c r="V16" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-5.5471546997513146</v>
       </c>
     </row>
@@ -2588,19 +2980,19 @@
       <c r="Q17" s="11"/>
       <c r="R17" s="11"/>
       <c r="S17" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E17:I17)</f>
+        <f t="shared" si="2"/>
         <v>-4.5708052339626111</v>
       </c>
       <c r="T17" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0349622493824083E-2</v>
       </c>
       <c r="U17" s="46">
-        <f>T17/SUMIF(A:A,A17,T:T)</f>
+        <f t="shared" si="4"/>
         <v>2.2869513424378688E-6</v>
       </c>
       <c r="V17" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-12.988290918865804</v>
       </c>
     </row>
@@ -2641,19 +3033,19 @@
       <c r="Q18" s="11"/>
       <c r="R18" s="11"/>
       <c r="S18" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E18:I18)</f>
+        <f t="shared" si="2"/>
         <v>-5.8003764092237127</v>
       </c>
       <c r="T18" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.0264153602953398E-3</v>
       </c>
       <c r="U18" s="46">
-        <f>T18/SUMIF(A:A,A18,T:T)</f>
+        <f t="shared" si="4"/>
         <v>6.6874561609683157E-7</v>
       </c>
       <c r="V18" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-14.217862094126906</v>
       </c>
     </row>
@@ -2692,19 +3084,19 @@
       <c r="Q19" s="11"/>
       <c r="R19" s="11"/>
       <c r="S19" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E19:I19)</f>
+        <f t="shared" si="2"/>
         <v>-5</v>
       </c>
       <c r="T19" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.737946999085467E-3</v>
       </c>
       <c r="U19" s="46">
-        <f>T19/SUMIF(A:A,A19,T:T)</f>
+        <f t="shared" si="4"/>
         <v>1.4888810624763294E-6</v>
       </c>
       <c r="V19" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-13.417485684903193</v>
       </c>
     </row>
@@ -2745,19 +3137,19 @@
       <c r="Q20" s="11"/>
       <c r="R20" s="11"/>
       <c r="S20" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E20:I20)</f>
+        <f t="shared" si="2"/>
         <v>-3.1746902135545079</v>
       </c>
       <c r="T20" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.1807053337514812E-2</v>
       </c>
       <c r="U20" s="46">
-        <f>T20/SUMIF(A:A,A20,T:T)</f>
+        <f t="shared" si="4"/>
         <v>9.2380854287830038E-6</v>
       </c>
       <c r="V20" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-11.5921758984577</v>
       </c>
     </row>
@@ -2798,19 +3190,19 @@
       <c r="Q21" s="11"/>
       <c r="R21" s="11"/>
       <c r="S21" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E21:I21)</f>
+        <f t="shared" si="2"/>
         <v>-4.4042611702320347</v>
       </c>
       <c r="T21" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.2225135372932079E-2</v>
       </c>
       <c r="U21" s="46">
-        <f>T21/SUMIF(A:A,A21,T:T)</f>
+        <f t="shared" si="4"/>
         <v>2.7013825643684305E-6</v>
       </c>
       <c r="V21" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-12.821746855135228</v>
       </c>
     </row>
@@ -2851,19 +3243,19 @@
       <c r="Q22" s="11"/>
       <c r="R22" s="11"/>
       <c r="S22" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E22:I22)</f>
+        <f t="shared" si="2"/>
         <v>-4.4042613888156099</v>
       </c>
       <c r="T22" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.2225132700718575E-2</v>
       </c>
       <c r="U22" s="46">
-        <f>T22/SUMIF(A:A,A22,T:T)</f>
+        <f t="shared" si="4"/>
         <v>2.7013819738906363E-6</v>
       </c>
       <c r="V22" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-12.821747073718802</v>
       </c>
     </row>
@@ -2907,19 +3299,19 @@
       <c r="Q23" s="10"/>
       <c r="R23" s="10"/>
       <c r="S23" s="24">
-        <f>-SUMPRODUCT(E$5:I$5,E23:I23)</f>
+        <f t="shared" si="2"/>
         <v>8.4135595645353831</v>
       </c>
       <c r="T23" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4507.777713186324</v>
       </c>
       <c r="U23" s="48">
-        <f>T23/SUMIF(A:A,A23,T:T)</f>
+        <f t="shared" si="4"/>
         <v>0.9960823774500448</v>
       </c>
       <c r="V23" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-3.9253165345027822E-3</v>
       </c>
     </row>
@@ -2958,19 +3350,19 @@
       <c r="Q24" s="11"/>
       <c r="R24" s="11"/>
       <c r="S24" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E24:I24)</f>
+        <f t="shared" si="2"/>
         <v>2.8703309851518783</v>
       </c>
       <c r="T24" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17.642856757169465</v>
       </c>
       <c r="U24" s="46">
-        <f>T24/SUMIF(A:A,A24,T:T)</f>
+        <f t="shared" si="4"/>
         <v>3.8985371111544776E-3</v>
       </c>
       <c r="V24" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-5.5471538959180071</v>
       </c>
     </row>
@@ -3011,19 +3403,19 @@
       <c r="Q25" s="11"/>
       <c r="R25" s="11"/>
       <c r="S25" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E25:I25)</f>
+        <f t="shared" si="2"/>
         <v>-4.5708052339626111</v>
       </c>
       <c r="T25" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0349622493824083E-2</v>
       </c>
       <c r="U25" s="46">
-        <f>T25/SUMIF(A:A,A25,T:T)</f>
+        <f t="shared" si="4"/>
         <v>2.2869531807662674E-6</v>
       </c>
       <c r="V25" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-12.988290115032497</v>
       </c>
     </row>
@@ -3064,19 +3456,19 @@
       <c r="Q26" s="11"/>
       <c r="R26" s="11"/>
       <c r="S26" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E26:I26)</f>
+        <f t="shared" si="2"/>
         <v>-5.8003761906401374</v>
       </c>
       <c r="T26" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.0264160218201018E-3</v>
       </c>
       <c r="U26" s="46">
-        <f>T26/SUMIF(A:A,A26,T:T)</f>
+        <f t="shared" si="4"/>
         <v>6.6874629983398882E-7</v>
       </c>
       <c r="V26" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-14.217861071710024</v>
       </c>
     </row>
@@ -3115,19 +3507,19 @@
       <c r="Q27" s="11"/>
       <c r="R27" s="11"/>
       <c r="S27" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E27:I27)</f>
+        <f t="shared" si="2"/>
         <v>-5</v>
       </c>
       <c r="T27" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.737946999085467E-3</v>
       </c>
       <c r="U27" s="46">
-        <f>T27/SUMIF(A:A,A27,T:T)</f>
+        <f t="shared" si="4"/>
         <v>1.4888822592889981E-6</v>
       </c>
       <c r="V27" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-13.417484881069885</v>
       </c>
     </row>
@@ -3168,19 +3560,19 @@
       <c r="Q28" s="11"/>
       <c r="R28" s="11"/>
       <c r="S28" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E28:I28)</f>
+        <f t="shared" si="2"/>
         <v>-3.1746905328662387</v>
       </c>
       <c r="T28" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.1807039988034381E-2</v>
       </c>
       <c r="U28" s="46">
-        <f>T28/SUMIF(A:A,A28,T:T)</f>
+        <f t="shared" si="4"/>
         <v>9.2380899048357991E-6</v>
       </c>
       <c r="V28" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-11.592175413936124</v>
       </c>
     </row>
@@ -3221,19 +3613,19 @@
       <c r="Q29" s="11"/>
       <c r="R29" s="11"/>
       <c r="S29" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E29:I29)</f>
+        <f t="shared" si="2"/>
         <v>-4.4042614895437637</v>
       </c>
       <c r="T29" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.2225131469303589E-2</v>
       </c>
       <c r="U29" s="46">
-        <f>T29/SUMIF(A:A,A29,T:T)</f>
+        <f t="shared" si="4"/>
         <v>2.7013838732468897E-6</v>
       </c>
       <c r="V29" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-12.821746370613649</v>
       </c>
     </row>
@@ -3274,19 +3666,19 @@
       <c r="Q30" s="11"/>
       <c r="R30" s="11"/>
       <c r="S30" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E30:I30)</f>
+        <f t="shared" si="2"/>
         <v>-4.404261708127339</v>
       </c>
       <c r="T30" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.2225128797090937E-2</v>
       </c>
       <c r="U30" s="46">
-        <f>T30/SUMIF(A:A,A30,T:T)</f>
+        <f t="shared" si="4"/>
         <v>2.7013832827688093E-6</v>
       </c>
       <c r="V30" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-12.821746589197225</v>
       </c>
     </row>
@@ -3328,19 +3720,19 @@
       <c r="Q31" s="10"/>
       <c r="R31" s="10"/>
       <c r="S31" s="24">
-        <f>-SUMPRODUCT(E$5:I$5,E31:I31)</f>
+        <f t="shared" si="2"/>
         <v>2.8703309851518783</v>
       </c>
       <c r="T31" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17.642856757169465</v>
       </c>
       <c r="U31" s="48">
-        <f>T31/SUMIF(A:A,A31,T:T)</f>
+        <f t="shared" si="4"/>
         <v>0.9986824223234243</v>
       </c>
       <c r="V31" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-1.3184464452399166E-3</v>
       </c>
     </row>
@@ -3381,19 +3773,19 @@
       <c r="Q32" s="11"/>
       <c r="R32" s="11"/>
       <c r="S32" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E32:I32)</f>
+        <f t="shared" si="2"/>
         <v>-4.5708052339626111</v>
       </c>
       <c r="T32" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0349622493824083E-2</v>
       </c>
       <c r="U32" s="46">
-        <f>T32/SUMIF(A:A,A32,T:T)</f>
+        <f t="shared" si="4"/>
         <v>5.8584537666016236E-4</v>
       </c>
       <c r="V32" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-7.4424546655597288</v>
       </c>
     </row>
@@ -3434,19 +3826,19 @@
       <c r="Q33" s="11"/>
       <c r="R33" s="11"/>
       <c r="S33" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E33:I33)</f>
+        <f t="shared" si="2"/>
         <v>-5.8003761906401374</v>
       </c>
       <c r="T33" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.0264160218201018E-3</v>
       </c>
       <c r="U33" s="46">
-        <f>T33/SUMIF(A:A,A33,T:T)</f>
+        <f t="shared" si="4"/>
         <v>1.7131173965925371E-4</v>
       </c>
       <c r="V33" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-8.6720256222372551</v>
       </c>
     </row>
@@ -3487,19 +3879,19 @@
       <c r="Q34" s="11"/>
       <c r="R34" s="11"/>
       <c r="S34" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E34:I34)</f>
+        <f t="shared" si="2"/>
         <v>-5.8003764092237127</v>
       </c>
       <c r="T34" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.0264153602953398E-3</v>
       </c>
       <c r="U34" s="46">
-        <f>T34/SUMIF(A:A,A34,T:T)</f>
+        <f t="shared" si="4"/>
         <v>1.7131170221332528E-4</v>
       </c>
       <c r="V34" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-8.6720258408208313</v>
       </c>
     </row>
@@ -3538,19 +3930,19 @@
       <c r="Q35" s="11"/>
       <c r="R35" s="11"/>
       <c r="S35" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E35:I35)</f>
+        <f t="shared" si="2"/>
         <v>-5</v>
       </c>
       <c r="T35" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.737946999085467E-3</v>
       </c>
       <c r="U35" s="46">
-        <f>T35/SUMIF(A:A,A35,T:T)</f>
+        <f t="shared" si="4"/>
         <v>3.8140474205227868E-4</v>
       </c>
       <c r="V35" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-7.8716494315971186</v>
       </c>
     </row>
@@ -3591,19 +3983,19 @@
       <c r="Q36" s="11"/>
       <c r="R36" s="11"/>
       <c r="S36" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E36:I36)</f>
+        <f t="shared" si="2"/>
         <v>-8.9021063960823064</v>
       </c>
       <c r="T36" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3610193974158367E-4</v>
       </c>
       <c r="U36" s="46">
-        <f>T36/SUMIF(A:A,A36,T:T)</f>
+        <f t="shared" si="4"/>
         <v>7.7041159906718126E-6</v>
       </c>
       <c r="V36" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-11.773755827679425</v>
       </c>
     </row>
@@ -3645,19 +4037,19 @@
       <c r="Q37" s="10"/>
       <c r="R37" s="10"/>
       <c r="S37" s="24">
-        <f>-SUMPRODUCT(E$5:I$5,E37:I37)</f>
+        <f t="shared" si="2"/>
         <v>2.8703309851518783</v>
       </c>
       <c r="T37" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17.642856757169465</v>
       </c>
       <c r="U37" s="48">
-        <f>T37/SUMIF(A:A,A37,T:T)</f>
+        <f t="shared" si="4"/>
         <v>0.99825732758791419</v>
       </c>
       <c r="V37" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-1.7441926320740813E-3</v>
       </c>
     </row>
@@ -3700,19 +4092,19 @@
       <c r="Q38" s="11"/>
       <c r="R38" s="11"/>
       <c r="S38" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E38:I38)</f>
+        <f t="shared" si="2"/>
         <v>-4.5613299361580717</v>
       </c>
       <c r="T38" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0448154321129497E-2</v>
       </c>
       <c r="U38" s="46">
-        <f>T38/SUMIF(A:A,A38,T:T)</f>
+        <f t="shared" si="4"/>
         <v>5.9117107588590892E-4</v>
       </c>
       <c r="V38" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-7.4334051139420243</v>
       </c>
     </row>
@@ -3753,19 +4145,19 @@
       <c r="Q39" s="11"/>
       <c r="R39" s="11"/>
       <c r="S39" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E39:I39)</f>
+        <f t="shared" si="2"/>
         <v>-5</v>
       </c>
       <c r="T39" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.737946999085467E-3</v>
       </c>
       <c r="U39" s="46">
-        <f>T39/SUMIF(A:A,A39,T:T)</f>
+        <f t="shared" si="4"/>
         <v>3.8124239499948105E-4</v>
       </c>
       <c r="V39" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-7.8720751777839526</v>
       </c>
     </row>
@@ -3806,19 +4198,19 @@
       <c r="Q40" s="11"/>
       <c r="R40" s="11"/>
       <c r="S40" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E40:I40)</f>
+        <f t="shared" si="2"/>
         <v>-5</v>
       </c>
       <c r="T40" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.737946999085467E-3</v>
       </c>
       <c r="U40" s="46">
-        <f>T40/SUMIF(A:A,A40,T:T)</f>
+        <f t="shared" si="4"/>
         <v>3.8124239499948105E-4</v>
       </c>
       <c r="V40" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-7.8720751777839526</v>
       </c>
     </row>
@@ -3859,19 +4251,19 @@
       <c r="Q41" s="11"/>
       <c r="R41" s="11"/>
       <c r="S41" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E41:I41)</f>
+        <f t="shared" si="2"/>
         <v>-5</v>
       </c>
       <c r="T41" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.737946999085467E-3</v>
       </c>
       <c r="U41" s="46">
-        <f>T41/SUMIF(A:A,A41,T:T)</f>
+        <f t="shared" si="4"/>
         <v>3.8124239499948105E-4</v>
       </c>
       <c r="V41" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-7.8720751777839526</v>
       </c>
     </row>
@@ -3914,19 +4306,19 @@
       <c r="Q42" s="11"/>
       <c r="R42" s="11"/>
       <c r="S42" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E42:I42)</f>
+        <f t="shared" si="2"/>
         <v>-8.8926310982777679</v>
       </c>
       <c r="T42" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3739767519768854E-4</v>
       </c>
       <c r="U42" s="46">
-        <f>T42/SUMIF(A:A,A42,T:T)</f>
+        <f t="shared" si="4"/>
         <v>7.7741512016697815E-6</v>
       </c>
       <c r="V42" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-11.76470627606172</v>
       </c>
     </row>
@@ -3970,19 +4362,19 @@
       <c r="Q43" s="9"/>
       <c r="R43" s="10"/>
       <c r="S43" s="24">
-        <f>-SUMPRODUCT(E$5:I$5,E43:I43)</f>
+        <f t="shared" si="2"/>
         <v>12.209402176222341</v>
       </c>
       <c r="T43" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>200667.01594726875</v>
       </c>
       <c r="U43" s="48">
-        <f>T43/SUMIF(A:A,A43,T:T)</f>
+        <f t="shared" si="4"/>
         <v>0.99991201646458683</v>
       </c>
       <c r="V43" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-8.7987406191468681E-5</v>
       </c>
     </row>
@@ -4025,19 +4417,19 @@
       <c r="P44" s="11"/>
       <c r="R44" s="11"/>
       <c r="S44" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E44:I44)</f>
+        <f t="shared" si="2"/>
         <v>-4.2753356896955079</v>
       </c>
       <c r="T44" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3907379371309063E-2</v>
       </c>
       <c r="U44" s="46">
-        <f>T44/SUMIF(A:A,A44,T:T)</f>
+        <f t="shared" si="4"/>
         <v>6.9299658866497019E-8</v>
       </c>
       <c r="V44" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-16.48482585332404</v>
       </c>
     </row>
@@ -4078,19 +4470,19 @@
       <c r="P45" s="11"/>
       <c r="R45" s="11"/>
       <c r="S45" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E45:I45)</f>
+        <f t="shared" si="2"/>
         <v>2.8703309851518783</v>
       </c>
       <c r="T45" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17.642856757169465</v>
       </c>
       <c r="U45" s="46">
-        <f>T45/SUMIF(A:A,A45,T:T)</f>
+        <f t="shared" si="4"/>
         <v>8.7913324434410079E-5</v>
       </c>
       <c r="V45" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-9.3391591784766543</v>
       </c>
     </row>
@@ -4133,19 +4525,19 @@
       <c r="P46" s="11"/>
       <c r="R46" s="11"/>
       <c r="S46" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E46:I46)</f>
+        <f t="shared" si="2"/>
         <v>-8.6066368518152032</v>
       </c>
       <c r="T46" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.8288795656911646E-4</v>
       </c>
       <c r="U46" s="46">
-        <f>T46/SUMIF(A:A,A46,T:T)</f>
+        <f t="shared" si="4"/>
         <v>9.1132000232747791E-10</v>
       </c>
       <c r="V46" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-20.816127015443737</v>
       </c>
     </row>
@@ -4189,19 +4581,19 @@
       <c r="Q47" s="37"/>
       <c r="R47" s="33"/>
       <c r="S47" s="35">
-        <f>-SUMPRODUCT(E$5:I$5,E47:I47)</f>
+        <f t="shared" si="2"/>
         <v>11.847569292910084</v>
       </c>
       <c r="T47" s="36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>139744.25665753122</v>
       </c>
       <c r="U47" s="49">
-        <f>T47/SUMIF(A:A,A47,T:T)</f>
+        <f t="shared" si="4"/>
         <v>0.90131647993849029</v>
       </c>
       <c r="V47" s="35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-0.10389882895530239</v>
       </c>
     </row>
@@ -4243,19 +4635,19 @@
       <c r="P48" s="11"/>
       <c r="Q48" s="11"/>
       <c r="S48" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E48:I48)</f>
+        <f t="shared" si="2"/>
         <v>9.6344770300004949</v>
       </c>
       <c r="T48" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15282.704299317336</v>
       </c>
       <c r="U48" s="46">
-        <f>T48/SUMIF(A:A,A48,T:T)</f>
+        <f t="shared" si="4"/>
         <v>9.8569727103408528E-2</v>
       </c>
       <c r="V48" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-2.3169910918648915</v>
       </c>
     </row>
@@ -4295,19 +4687,19 @@
       <c r="P49" s="11"/>
       <c r="Q49" s="11"/>
       <c r="S49" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E49:I49)</f>
+        <f t="shared" si="2"/>
         <v>2.8703309851518783</v>
       </c>
       <c r="T49" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17.642856757169465</v>
       </c>
       <c r="U49" s="46">
-        <f>T49/SUMIF(A:A,A49,T:T)</f>
+        <f t="shared" si="4"/>
         <v>1.1379213664144525E-4</v>
       </c>
       <c r="V49" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-9.0811371367135081</v>
       </c>
     </row>
@@ -4349,19 +4741,19 @@
       <c r="P50" s="11"/>
       <c r="Q50" s="11"/>
       <c r="S50" s="22">
-        <f>-SUMPRODUCT(E$5:I$5,E50:I50)</f>
+        <f t="shared" si="2"/>
         <v>-8.9684697351274618</v>
       </c>
       <c r="T50" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.2736294214432331E-4</v>
       </c>
       <c r="U50" s="46">
-        <f>T50/SUMIF(A:A,A50,T:T)</f>
+        <f t="shared" si="4"/>
         <v>8.2146001155135472E-10</v>
       </c>
       <c r="V50" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-20.919937856992849</v>
       </c>
     </row>
@@ -4396,12 +4788,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{460165A2-3E40-4443-8001-FC6267ACCC55}">
   <dimension ref="A2:Z56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="AA8" sqref="AA8"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7789,7 +8181,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EE4A12C-F81F-5344-95C6-9D393BB4DD30}">
   <dimension ref="A1:X50"/>
   <sheetViews>
@@ -11323,7 +11715,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B73D90-E08E-464C-8F42-5EA90A6C7273}">
   <dimension ref="A1:Z57"/>
   <sheetViews>
@@ -11769,7 +12161,7 @@
         <v>4.6033540293598718E-10</v>
       </c>
       <c r="V8" s="24">
-        <f>U8/SUMIF(A:A,A8,U:U)</f>
+        <f t="shared" ref="V8:V39" si="3">U8/SUMIF(A:A,A8,U:U)</f>
         <v>2.7960732692348036E-7</v>
       </c>
       <c r="W8" s="24">
@@ -11840,23 +12232,23 @@
         <v>0</v>
       </c>
       <c r="T9" s="55">
-        <f t="shared" ref="T9:T57" si="3">-SUMPRODUCT(F$6:S$6,F9:S9)</f>
+        <f t="shared" ref="T9:T57" si="4">-SUMPRODUCT(F$6:S$6,F9:S9)</f>
         <v>-7.1066963640451837</v>
       </c>
       <c r="U9" s="56">
-        <f t="shared" ref="U9:U57" si="4">EXP(T9)</f>
+        <f t="shared" ref="U9:U57" si="5">EXP(T9)</f>
         <v>8.1959817848556589E-4</v>
       </c>
       <c r="V9" s="55">
-        <f>U9/SUMIF(A:A,A9,U:U)</f>
+        <f t="shared" si="3"/>
         <v>0.49782322709941496</v>
       </c>
       <c r="W9" s="55" t="str">
-        <f t="shared" ref="W9:W57" si="5">IF(C9=C8,"",SUMIF(C:C,C9,V:V))</f>
+        <f t="shared" ref="W9:W57" si="6">IF(C9=C8,"",SUMIF(C:C,C9,V:V))</f>
         <v/>
       </c>
       <c r="X9" s="58" t="str">
-        <f t="shared" ref="X9:X57" si="6">IF(W9="","NA",LN(W9))</f>
+        <f t="shared" ref="X9:X57" si="7">IF(W9="","NA",LN(W9))</f>
         <v>NA</v>
       </c>
     </row>
@@ -11919,23 +12311,23 @@
         <v>0</v>
       </c>
       <c r="T10" s="55">
+        <f t="shared" si="4"/>
+        <v>-14.200484785906454</v>
+      </c>
+      <c r="U10" s="56">
+        <f t="shared" si="5"/>
+        <v>6.8046817304370684E-7</v>
+      </c>
+      <c r="V10" s="55">
         <f t="shared" si="3"/>
-        <v>-14.200484785906454</v>
-      </c>
-      <c r="U10" s="56">
-        <f t="shared" si="4"/>
-        <v>6.8046817304370684E-7</v>
-      </c>
-      <c r="V10" s="55">
-        <f>U10/SUMIF(A:A,A10,U:U)</f>
         <v>4.133157817273347E-4</v>
       </c>
       <c r="W10" s="55" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="X10" s="58" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
     </row>
@@ -11998,23 +12390,23 @@
         <v>0</v>
       </c>
       <c r="T11" s="22">
+        <f t="shared" si="4"/>
+        <v>-7.1022475406298931</v>
+      </c>
+      <c r="U11" s="25">
+        <f t="shared" si="5"/>
+        <v>8.2325254885008302E-4</v>
+      </c>
+      <c r="V11" s="22">
         <f t="shared" si="3"/>
-        <v>-7.1022475406298931</v>
-      </c>
-      <c r="U11" s="25">
-        <f t="shared" si="4"/>
-        <v>8.2325254885008302E-4</v>
-      </c>
-      <c r="V11" s="22">
-        <f>U11/SUMIF(A:A,A11,U:U)</f>
         <v>0.50004288850867029</v>
       </c>
       <c r="W11" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.50004288850867029</v>
       </c>
       <c r="X11" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.69306140722124276</v>
       </c>
       <c r="Y11" s="2" t="s">
@@ -12084,23 +12476,23 @@
         <v>0</v>
       </c>
       <c r="T12" s="22">
+        <f t="shared" si="4"/>
+        <v>-14.200484785906454</v>
+      </c>
+      <c r="U12" s="25">
+        <f t="shared" si="5"/>
+        <v>6.8046817304370684E-7</v>
+      </c>
+      <c r="V12" s="22">
         <f t="shared" si="3"/>
-        <v>-14.200484785906454</v>
-      </c>
-      <c r="U12" s="25">
-        <f t="shared" si="4"/>
-        <v>6.8046817304370684E-7</v>
-      </c>
-      <c r="V12" s="22">
-        <f>U12/SUMIF(A:A,A12,U:U)</f>
         <v>4.133157817273347E-4</v>
       </c>
       <c r="W12" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.133157817273347E-4</v>
       </c>
       <c r="X12" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-7.7912986524978036</v>
       </c>
       <c r="Y12" s="2" t="s">
@@ -12170,23 +12562,23 @@
         <v>0</v>
       </c>
       <c r="T13" s="22">
+        <f t="shared" si="4"/>
+        <v>-14.200484785906454</v>
+      </c>
+      <c r="U13" s="25">
+        <f t="shared" si="5"/>
+        <v>6.8046817304370684E-7</v>
+      </c>
+      <c r="V13" s="22">
         <f t="shared" si="3"/>
-        <v>-14.200484785906454</v>
-      </c>
-      <c r="U13" s="25">
-        <f t="shared" si="4"/>
-        <v>6.8046817304370684E-7</v>
-      </c>
-      <c r="V13" s="22">
-        <f>U13/SUMIF(A:A,A13,U:U)</f>
         <v>4.133157817273347E-4</v>
       </c>
       <c r="W13" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.133157817273347E-4</v>
       </c>
       <c r="X13" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-7.7912986524978036</v>
       </c>
     </row>
@@ -12249,23 +12641,23 @@
         <v>0</v>
       </c>
       <c r="T14" s="22">
+        <f t="shared" si="4"/>
+        <v>-14.200484785906454</v>
+      </c>
+      <c r="U14" s="25">
+        <f t="shared" si="5"/>
+        <v>6.8046817304370684E-7</v>
+      </c>
+      <c r="V14" s="22">
         <f t="shared" si="3"/>
-        <v>-14.200484785906454</v>
-      </c>
-      <c r="U14" s="25">
-        <f t="shared" si="4"/>
-        <v>6.8046817304370684E-7</v>
-      </c>
-      <c r="V14" s="22">
-        <f>U14/SUMIF(A:A,A14,U:U)</f>
         <v>4.133157817273347E-4</v>
       </c>
       <c r="W14" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.133157817273347E-4</v>
       </c>
       <c r="X14" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-7.7912986524978036</v>
       </c>
     </row>
@@ -12328,23 +12720,23 @@
         <v>0</v>
       </c>
       <c r="T15" s="22">
+        <f t="shared" si="4"/>
+        <v>-15.14881134250904</v>
+      </c>
+      <c r="U15" s="25">
+        <f t="shared" si="5"/>
+        <v>2.6360571802287428E-7</v>
+      </c>
+      <c r="V15" s="22">
         <f t="shared" si="3"/>
-        <v>-15.14881134250904</v>
-      </c>
-      <c r="U15" s="25">
-        <f t="shared" si="4"/>
-        <v>2.6360571802287428E-7</v>
-      </c>
-      <c r="V15" s="22">
-        <f>U15/SUMIF(A:A,A15,U:U)</f>
         <v>1.6011388589282571E-4</v>
       </c>
       <c r="W15" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.6011388589282571E-4</v>
       </c>
       <c r="X15" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-8.7396252091003905</v>
       </c>
     </row>
@@ -12407,23 +12799,23 @@
         <v>0</v>
       </c>
       <c r="T16" s="22">
+        <f t="shared" si="4"/>
+        <v>-15.14881134250904</v>
+      </c>
+      <c r="U16" s="25">
+        <f t="shared" si="5"/>
+        <v>2.6360571802287428E-7</v>
+      </c>
+      <c r="V16" s="22">
         <f t="shared" si="3"/>
-        <v>-15.14881134250904</v>
-      </c>
-      <c r="U16" s="25">
-        <f t="shared" si="4"/>
-        <v>2.6360571802287428E-7</v>
-      </c>
-      <c r="V16" s="22">
-        <f>U16/SUMIF(A:A,A16,U:U)</f>
         <v>1.6011388589282571E-4</v>
       </c>
       <c r="W16" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.6011388589282571E-4</v>
       </c>
       <c r="X16" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-8.7396252091003905</v>
       </c>
     </row>
@@ -12486,23 +12878,23 @@
         <v>0</v>
       </c>
       <c r="T17" s="22">
+        <f t="shared" si="4"/>
+        <v>-15.14881134250904</v>
+      </c>
+      <c r="U17" s="25">
+        <f t="shared" si="5"/>
+        <v>2.6360571802287428E-7</v>
+      </c>
+      <c r="V17" s="22">
         <f t="shared" si="3"/>
-        <v>-15.14881134250904</v>
-      </c>
-      <c r="U17" s="25">
-        <f t="shared" si="4"/>
-        <v>2.6360571802287428E-7</v>
-      </c>
-      <c r="V17" s="22">
-        <f>U17/SUMIF(A:A,A17,U:U)</f>
         <v>1.6011388589282571E-4</v>
       </c>
       <c r="W17" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.6011388589282571E-4</v>
       </c>
       <c r="X17" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-8.7396252091003905</v>
       </c>
     </row>
@@ -12565,23 +12957,23 @@
         <v>1</v>
       </c>
       <c r="T18" s="24">
+        <f t="shared" si="4"/>
+        <v>-21.499065755319151</v>
+      </c>
+      <c r="U18" s="27">
+        <f t="shared" si="5"/>
+        <v>4.6033540293598718E-10</v>
+      </c>
+      <c r="V18" s="24">
         <f t="shared" si="3"/>
-        <v>-21.499065755319151</v>
-      </c>
-      <c r="U18" s="27">
-        <f t="shared" si="4"/>
-        <v>4.6033540293598718E-10</v>
-      </c>
-      <c r="V18" s="24">
-        <f>U18/SUMIF(A:A,A18,U:U)</f>
         <v>5.6027686299772719E-7</v>
       </c>
       <c r="W18" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.99753944610011858</v>
       </c>
       <c r="X18" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-2.4635860374750593E-3</v>
       </c>
     </row>
@@ -12644,23 +13036,23 @@
         <v>0</v>
       </c>
       <c r="T19" s="55">
+        <f t="shared" si="4"/>
+        <v>-7.1066963640451837</v>
+      </c>
+      <c r="U19" s="56">
+        <f t="shared" si="5"/>
+        <v>8.1959817848556589E-4</v>
+      </c>
+      <c r="V19" s="55">
         <f t="shared" si="3"/>
-        <v>-7.1066963640451837</v>
-      </c>
-      <c r="U19" s="56">
-        <f t="shared" si="4"/>
-        <v>8.1959817848556589E-4</v>
-      </c>
-      <c r="V19" s="55">
-        <f>U19/SUMIF(A:A,A19,U:U)</f>
         <v>0.99753765066033684</v>
       </c>
       <c r="W19" s="55" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="X19" s="58" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
     </row>
@@ -12723,23 +13115,23 @@
         <v>0</v>
       </c>
       <c r="T20" s="55">
+        <f t="shared" si="4"/>
+        <v>-20.708538656754584</v>
+      </c>
+      <c r="U20" s="56">
+        <f t="shared" si="5"/>
+        <v>1.014836159438483E-9</v>
+      </c>
+      <c r="V20" s="55">
         <f t="shared" si="3"/>
-        <v>-20.708538656754584</v>
-      </c>
-      <c r="U20" s="56">
-        <f t="shared" si="4"/>
-        <v>1.014836159438483E-9</v>
-      </c>
-      <c r="V20" s="55">
-        <f>U20/SUMIF(A:A,A20,U:U)</f>
         <v>1.2351629186902247E-6</v>
       </c>
       <c r="W20" s="55" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="X20" s="58" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
     </row>
@@ -12802,23 +13194,23 @@
         <v>0</v>
       </c>
       <c r="T21" s="22">
+        <f t="shared" si="4"/>
+        <v>-13.610301411478023</v>
+      </c>
+      <c r="U21" s="25">
+        <f t="shared" si="5"/>
+        <v>1.2277818243665275E-6</v>
+      </c>
+      <c r="V21" s="22">
         <f t="shared" si="3"/>
-        <v>-13.610301411478023</v>
-      </c>
-      <c r="U21" s="25">
-        <f t="shared" si="4"/>
-        <v>1.2277818243665275E-6</v>
-      </c>
-      <c r="V21" s="22">
-        <f>U21/SUMIF(A:A,A21,U:U)</f>
         <v>1.4943403105960144E-3</v>
       </c>
       <c r="W21" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.4943403105960144E-3</v>
       </c>
       <c r="X21" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-6.5060704333403896</v>
       </c>
     </row>
@@ -12881,23 +13273,23 @@
         <v>0</v>
       </c>
       <c r="T22" s="22">
+        <f t="shared" si="4"/>
+        <v>-20.708538656754584</v>
+      </c>
+      <c r="U22" s="25">
+        <f t="shared" si="5"/>
+        <v>1.014836159438483E-9</v>
+      </c>
+      <c r="V22" s="22">
         <f t="shared" si="3"/>
-        <v>-20.708538656754584</v>
-      </c>
-      <c r="U22" s="25">
-        <f t="shared" si="4"/>
-        <v>1.014836159438483E-9</v>
-      </c>
-      <c r="V22" s="22">
-        <f>U22/SUMIF(A:A,A22,U:U)</f>
         <v>1.2351629186902247E-6</v>
       </c>
       <c r="W22" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.2351629186902247E-6</v>
       </c>
       <c r="X22" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-13.60430767861695</v>
       </c>
     </row>
@@ -12960,23 +13352,23 @@
         <v>0</v>
       </c>
       <c r="T23" s="22">
+        <f t="shared" si="4"/>
+        <v>-20.708538656754584</v>
+      </c>
+      <c r="U23" s="25">
+        <f t="shared" si="5"/>
+        <v>1.014836159438483E-9</v>
+      </c>
+      <c r="V23" s="22">
         <f t="shared" si="3"/>
-        <v>-20.708538656754584</v>
-      </c>
-      <c r="U23" s="25">
-        <f t="shared" si="4"/>
-        <v>1.014836159438483E-9</v>
-      </c>
-      <c r="V23" s="22">
-        <f>U23/SUMIF(A:A,A23,U:U)</f>
         <v>1.2351629186902247E-6</v>
       </c>
       <c r="W23" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.2351629186902247E-6</v>
       </c>
       <c r="X23" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-13.60430767861695</v>
       </c>
     </row>
@@ -13039,23 +13431,23 @@
         <v>0</v>
       </c>
       <c r="T24" s="22">
+        <f t="shared" si="4"/>
+        <v>-20.708538656754584</v>
+      </c>
+      <c r="U24" s="25">
+        <f t="shared" si="5"/>
+        <v>1.014836159438483E-9</v>
+      </c>
+      <c r="V24" s="22">
         <f t="shared" si="3"/>
-        <v>-20.708538656754584</v>
-      </c>
-      <c r="U24" s="25">
-        <f t="shared" si="4"/>
-        <v>1.014836159438483E-9</v>
-      </c>
-      <c r="V24" s="22">
-        <f>U24/SUMIF(A:A,A24,U:U)</f>
         <v>1.2351629186902247E-6</v>
       </c>
       <c r="W24" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.2351629186902247E-6</v>
       </c>
       <c r="X24" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-13.60430767861695</v>
       </c>
     </row>
@@ -13118,23 +13510,23 @@
         <v>0</v>
       </c>
       <c r="T25" s="22">
+        <f t="shared" si="4"/>
+        <v>-15.14881134250904</v>
+      </c>
+      <c r="U25" s="25">
+        <f t="shared" si="5"/>
+        <v>2.6360571802287428E-7</v>
+      </c>
+      <c r="V25" s="22">
         <f t="shared" si="3"/>
-        <v>-15.14881134250904</v>
-      </c>
-      <c r="U25" s="25">
-        <f t="shared" si="4"/>
-        <v>2.6360571802287428E-7</v>
-      </c>
-      <c r="V25" s="22">
-        <f>U25/SUMIF(A:A,A25,U:U)</f>
         <v>3.2083603350980383E-4</v>
       </c>
       <c r="W25" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.2083603350980383E-4</v>
       </c>
       <c r="X25" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-8.0445803643714058</v>
       </c>
     </row>
@@ -13197,23 +13589,23 @@
         <v>0</v>
       </c>
       <c r="T26" s="22">
+        <f t="shared" si="4"/>
+        <v>-15.14881134250904</v>
+      </c>
+      <c r="U26" s="25">
+        <f t="shared" si="5"/>
+        <v>2.6360571802287428E-7</v>
+      </c>
+      <c r="V26" s="22">
         <f t="shared" si="3"/>
-        <v>-15.14881134250904</v>
-      </c>
-      <c r="U26" s="25">
-        <f t="shared" si="4"/>
-        <v>2.6360571802287428E-7</v>
-      </c>
-      <c r="V26" s="22">
-        <f>U26/SUMIF(A:A,A26,U:U)</f>
         <v>3.2083603350980383E-4</v>
       </c>
       <c r="W26" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.2083603350980383E-4</v>
       </c>
       <c r="X26" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-8.0445803643714058</v>
       </c>
     </row>
@@ -13276,23 +13668,23 @@
         <v>0</v>
       </c>
       <c r="T27" s="22">
+        <f t="shared" si="4"/>
+        <v>-15.14881134250904</v>
+      </c>
+      <c r="U27" s="25">
+        <f t="shared" si="5"/>
+        <v>2.6360571802287428E-7</v>
+      </c>
+      <c r="V27" s="22">
         <f t="shared" si="3"/>
-        <v>-15.14881134250904</v>
-      </c>
-      <c r="U27" s="25">
-        <f t="shared" si="4"/>
-        <v>2.6360571802287428E-7</v>
-      </c>
-      <c r="V27" s="22">
-        <f>U27/SUMIF(A:A,A27,U:U)</f>
         <v>3.2083603350980383E-4</v>
       </c>
       <c r="W27" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.2083603350980383E-4</v>
       </c>
       <c r="X27" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-8.0445803643714058</v>
       </c>
     </row>
@@ -13355,23 +13747,23 @@
         <v>1</v>
       </c>
       <c r="T28" s="24">
+        <f t="shared" si="4"/>
+        <v>-21.499065755319151</v>
+      </c>
+      <c r="U28" s="27">
+        <f t="shared" si="5"/>
+        <v>4.6033540293598718E-10</v>
+      </c>
+      <c r="V28" s="24">
         <f t="shared" si="3"/>
-        <v>-21.499065755319151</v>
-      </c>
-      <c r="U28" s="27">
-        <f t="shared" si="4"/>
-        <v>4.6033540293598718E-10</v>
-      </c>
-      <c r="V28" s="24">
-        <f>U28/SUMIF(A:A,A28,U:U)</f>
         <v>5.6037199704480108E-7</v>
       </c>
       <c r="W28" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.99770868669517265</v>
       </c>
       <c r="X28" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-2.2939423799487589E-3</v>
       </c>
     </row>
@@ -13434,23 +13826,23 @@
         <v>0</v>
       </c>
       <c r="T29" s="55">
+        <f t="shared" si="4"/>
+        <v>-7.1066963640451837</v>
+      </c>
+      <c r="U29" s="56">
+        <f t="shared" si="5"/>
+        <v>8.1959817848556589E-4</v>
+      </c>
+      <c r="V29" s="55">
         <f t="shared" si="3"/>
-        <v>-7.1066963640451837</v>
-      </c>
-      <c r="U29" s="56">
-        <f t="shared" si="4"/>
-        <v>8.1959817848556589E-4</v>
-      </c>
-      <c r="V29" s="55">
-        <f>U29/SUMIF(A:A,A29,U:U)</f>
         <v>0.99770703083660917</v>
       </c>
       <c r="W29" s="55" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="X29" s="58" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
     </row>
@@ -13513,23 +13905,23 @@
         <v>0</v>
       </c>
       <c r="T30" s="55">
+        <f t="shared" si="4"/>
+        <v>-20.828712702484943</v>
+      </c>
+      <c r="U30" s="56">
+        <f t="shared" si="5"/>
+        <v>8.9992228846260469E-10</v>
+      </c>
+      <c r="V30" s="55">
         <f t="shared" si="3"/>
-        <v>-20.828712702484943</v>
-      </c>
-      <c r="U30" s="56">
-        <f t="shared" si="4"/>
-        <v>8.9992228846260469E-10</v>
-      </c>
-      <c r="V30" s="55">
-        <f>U30/SUMIF(A:A,A30,U:U)</f>
         <v>1.0954865664352183E-6</v>
       </c>
       <c r="W30" s="55" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="X30" s="58" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
     </row>
@@ -13592,23 +13984,23 @@
         <v>0</v>
       </c>
       <c r="T31" s="22">
+        <f t="shared" si="4"/>
+        <v>-13.730475457208383</v>
+      </c>
+      <c r="U31" s="25">
+        <f t="shared" si="5"/>
+        <v>1.0887552821610829E-6</v>
+      </c>
+      <c r="V31" s="22">
         <f t="shared" si="3"/>
-        <v>-13.730475457208383</v>
-      </c>
-      <c r="U31" s="25">
-        <f t="shared" si="4"/>
-        <v>1.0887552821610829E-6</v>
-      </c>
-      <c r="V31" s="22">
-        <f>U31/SUMIF(A:A,A31,U:U)</f>
         <v>1.3253553123797467E-3</v>
       </c>
       <c r="W31" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.3253553123797467E-3</v>
       </c>
       <c r="X31" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-6.6260746952058938</v>
       </c>
     </row>
@@ -13671,23 +14063,23 @@
         <v>0</v>
       </c>
       <c r="T32" s="22">
+        <f t="shared" si="4"/>
+        <v>-20.828712702484943</v>
+      </c>
+      <c r="U32" s="25">
+        <f t="shared" si="5"/>
+        <v>8.9992228846260469E-10</v>
+      </c>
+      <c r="V32" s="22">
         <f t="shared" si="3"/>
-        <v>-20.828712702484943</v>
-      </c>
-      <c r="U32" s="25">
-        <f t="shared" si="4"/>
-        <v>8.9992228846260469E-10</v>
-      </c>
-      <c r="V32" s="22">
-        <f>U32/SUMIF(A:A,A32,U:U)</f>
         <v>1.0954865664352183E-6</v>
       </c>
       <c r="W32" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.0954865664352183E-6</v>
       </c>
       <c r="X32" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-13.724311940482453</v>
       </c>
     </row>
@@ -13750,23 +14142,23 @@
         <v>0</v>
       </c>
       <c r="T33" s="22">
+        <f t="shared" si="4"/>
+        <v>-20.828712702484943</v>
+      </c>
+      <c r="U33" s="25">
+        <f t="shared" si="5"/>
+        <v>8.9992228846260469E-10</v>
+      </c>
+      <c r="V33" s="22">
         <f t="shared" si="3"/>
-        <v>-20.828712702484943</v>
-      </c>
-      <c r="U33" s="25">
-        <f t="shared" si="4"/>
-        <v>8.9992228846260469E-10</v>
-      </c>
-      <c r="V33" s="22">
-        <f>U33/SUMIF(A:A,A33,U:U)</f>
         <v>1.0954865664352183E-6</v>
       </c>
       <c r="W33" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.0954865664352183E-6</v>
       </c>
       <c r="X33" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-13.724311940482453</v>
       </c>
     </row>
@@ -13829,23 +14221,23 @@
         <v>0</v>
       </c>
       <c r="T34" s="22">
+        <f t="shared" si="4"/>
+        <v>-20.828712702484943</v>
+      </c>
+      <c r="U34" s="25">
+        <f t="shared" si="5"/>
+        <v>8.9992228846260469E-10</v>
+      </c>
+      <c r="V34" s="22">
         <f t="shared" si="3"/>
-        <v>-20.828712702484943</v>
-      </c>
-      <c r="U34" s="25">
-        <f t="shared" si="4"/>
-        <v>8.9992228846260469E-10</v>
-      </c>
-      <c r="V34" s="22">
-        <f>U34/SUMIF(A:A,A34,U:U)</f>
         <v>1.0954865664352183E-6</v>
       </c>
       <c r="W34" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.0954865664352183E-6</v>
       </c>
       <c r="X34" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-13.724311940482453</v>
       </c>
     </row>
@@ -13908,23 +14300,23 @@
         <v>0</v>
       </c>
       <c r="T35" s="22">
+        <f t="shared" si="4"/>
+        <v>-15.14881134250904</v>
+      </c>
+      <c r="U35" s="25">
+        <f t="shared" si="5"/>
+        <v>2.6360571802287428E-7</v>
+      </c>
+      <c r="V35" s="22">
         <f t="shared" si="3"/>
-        <v>-15.14881134250904</v>
-      </c>
-      <c r="U35" s="25">
-        <f t="shared" si="4"/>
-        <v>2.6360571802287428E-7</v>
-      </c>
-      <c r="V35" s="22">
-        <f>U35/SUMIF(A:A,A35,U:U)</f>
         <v>3.2089051091611969E-4</v>
       </c>
       <c r="W35" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.2089051091611969E-4</v>
       </c>
       <c r="X35" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-8.0444105805065504</v>
       </c>
     </row>
@@ -13987,23 +14379,23 @@
         <v>0</v>
       </c>
       <c r="T36" s="22">
+        <f t="shared" si="4"/>
+        <v>-15.14881134250904</v>
+      </c>
+      <c r="U36" s="25">
+        <f t="shared" si="5"/>
+        <v>2.6360571802287428E-7</v>
+      </c>
+      <c r="V36" s="22">
         <f t="shared" si="3"/>
-        <v>-15.14881134250904</v>
-      </c>
-      <c r="U36" s="25">
-        <f t="shared" si="4"/>
-        <v>2.6360571802287428E-7</v>
-      </c>
-      <c r="V36" s="22">
-        <f>U36/SUMIF(A:A,A36,U:U)</f>
         <v>3.2089051091611969E-4</v>
       </c>
       <c r="W36" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.2089051091611969E-4</v>
       </c>
       <c r="X36" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-8.0444105805065504</v>
       </c>
     </row>
@@ -14066,23 +14458,23 @@
         <v>0</v>
       </c>
       <c r="T37" s="22">
+        <f t="shared" si="4"/>
+        <v>-15.14881134250904</v>
+      </c>
+      <c r="U37" s="25">
+        <f t="shared" si="5"/>
+        <v>2.6360571802287428E-7</v>
+      </c>
+      <c r="V37" s="22">
         <f t="shared" si="3"/>
-        <v>-15.14881134250904</v>
-      </c>
-      <c r="U37" s="25">
-        <f t="shared" si="4"/>
-        <v>2.6360571802287428E-7</v>
-      </c>
-      <c r="V37" s="22">
-        <f>U37/SUMIF(A:A,A37,U:U)</f>
         <v>3.2089051091611969E-4</v>
       </c>
       <c r="W37" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.2089051091611969E-4</v>
       </c>
       <c r="X37" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-8.0444105805065504</v>
       </c>
     </row>
@@ -14145,23 +14537,23 @@
         <v>0</v>
       </c>
       <c r="T38" s="24">
+        <f t="shared" si="4"/>
+        <v>-8.459118768623132E-3</v>
+      </c>
+      <c r="U38" s="27">
+        <f t="shared" si="5"/>
+        <v>0.99157655890511187</v>
+      </c>
+      <c r="V38" s="24">
         <f t="shared" si="3"/>
-        <v>-8.459118768623132E-3</v>
-      </c>
-      <c r="U38" s="27">
-        <f t="shared" si="4"/>
-        <v>0.99157655890511187</v>
-      </c>
-      <c r="V38" s="24">
-        <f>U38/SUMIF(A:A,A38,U:U)</f>
         <v>0.99670438846830645</v>
       </c>
       <c r="W38" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.99670438846830645</v>
       </c>
       <c r="X38" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-3.3010540202191721E-3</v>
       </c>
     </row>
@@ -14224,23 +14616,23 @@
         <v>0</v>
       </c>
       <c r="T39" s="22">
+        <f t="shared" si="4"/>
+        <v>-7.1066963640451837</v>
+      </c>
+      <c r="U39" s="25">
+        <f t="shared" si="5"/>
+        <v>8.1959817848556589E-4</v>
+      </c>
+      <c r="V39" s="22">
         <f t="shared" si="3"/>
-        <v>-7.1066963640451837</v>
-      </c>
-      <c r="U39" s="25">
-        <f t="shared" si="4"/>
-        <v>8.1959817848556589E-4</v>
-      </c>
-      <c r="V39" s="22">
-        <f>U39/SUMIF(A:A,A39,U:U)</f>
         <v>8.2383664069187238E-4</v>
       </c>
       <c r="W39" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.2383664069187238E-4</v>
       </c>
       <c r="X39" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-7.1015382992967799</v>
       </c>
     </row>
@@ -14303,23 +14695,23 @@
         <v>0</v>
       </c>
       <c r="T40" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-7.1066963640451837</v>
       </c>
       <c r="U40" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.1959817848556589E-4</v>
       </c>
       <c r="V40" s="22">
-        <f>U40/SUMIF(A:A,A40,U:U)</f>
+        <f t="shared" ref="V40:V71" si="8">U40/SUMIF(A:A,A40,U:U)</f>
         <v>8.2383664069187238E-4</v>
       </c>
       <c r="W40" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.2383664069187238E-4</v>
       </c>
       <c r="X40" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-7.1015382992967799</v>
       </c>
     </row>
@@ -14382,23 +14774,23 @@
         <v>0</v>
       </c>
       <c r="T41" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-7.1066963640451837</v>
       </c>
       <c r="U41" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.1959817848556589E-4</v>
       </c>
       <c r="V41" s="22">
-        <f>U41/SUMIF(A:A,A41,U:U)</f>
+        <f t="shared" si="8"/>
         <v>8.2383664069187238E-4</v>
       </c>
       <c r="W41" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.2383664069187238E-4</v>
       </c>
       <c r="X41" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-7.1015382992967799</v>
       </c>
     </row>
@@ -14461,23 +14853,23 @@
         <v>0</v>
       </c>
       <c r="T42" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-7.1066963640451837</v>
       </c>
       <c r="U42" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.1959817848556589E-4</v>
       </c>
       <c r="V42" s="22">
-        <f>U42/SUMIF(A:A,A42,U:U)</f>
+        <f t="shared" si="8"/>
         <v>8.2383664069187238E-4</v>
       </c>
       <c r="W42" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.2383664069187238E-4</v>
       </c>
       <c r="X42" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-7.1015382992967799</v>
       </c>
     </row>
@@ -14540,23 +14932,23 @@
         <v>0</v>
       </c>
       <c r="T43" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-15.14881134250904</v>
       </c>
       <c r="U43" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.6360571802287428E-7</v>
       </c>
       <c r="V43" s="22">
-        <f>U43/SUMIF(A:A,A43,U:U)</f>
+        <f t="shared" si="8"/>
         <v>2.6496892611988438E-7</v>
       </c>
       <c r="W43" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.6496892611988438E-7</v>
       </c>
       <c r="X43" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-15.143653277760636</v>
       </c>
     </row>
@@ -14619,23 +15011,23 @@
         <v>0</v>
       </c>
       <c r="T44" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-7.1022475406298931</v>
       </c>
       <c r="U44" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.2325254885008302E-4</v>
       </c>
       <c r="V44" s="24">
-        <f>U44/SUMIF(A:A,A44,U:U)</f>
+        <f t="shared" si="8"/>
         <v>0.50041010103072492</v>
       </c>
       <c r="W44" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.50041010103072492</v>
       </c>
       <c r="X44" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.6923273146803941</v>
       </c>
     </row>
@@ -14698,23 +15090,23 @@
         <v>0</v>
       </c>
       <c r="T45" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-7.1066963640451837</v>
       </c>
       <c r="U45" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.1959817848556589E-4</v>
       </c>
       <c r="V45" s="22">
-        <f>U45/SUMIF(A:A,A45,U:U)</f>
+        <f t="shared" si="8"/>
         <v>0.49818880958636075</v>
       </c>
       <c r="W45" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.49818880958636075</v>
       </c>
       <c r="X45" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.69677613809568473</v>
       </c>
     </row>
@@ -14777,23 +15169,23 @@
         <v>0</v>
       </c>
       <c r="T46" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-14.200484785906454</v>
       </c>
       <c r="U46" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.8046817304370684E-7</v>
       </c>
       <c r="V46" s="22">
-        <f>U46/SUMIF(A:A,A46,U:U)</f>
+        <f t="shared" si="8"/>
         <v>4.1361930515322674E-4</v>
       </c>
       <c r="W46" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.1361930515322674E-4</v>
       </c>
       <c r="X46" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-7.7905645599569553</v>
       </c>
     </row>
@@ -14856,23 +15248,23 @@
         <v>0</v>
       </c>
       <c r="T47" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-14.200484785906454</v>
       </c>
       <c r="U47" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.8046817304370684E-7</v>
       </c>
       <c r="V47" s="22">
-        <f>U47/SUMIF(A:A,A47,U:U)</f>
+        <f t="shared" si="8"/>
         <v>4.1361930515322674E-4</v>
       </c>
       <c r="W47" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.1361930515322674E-4</v>
       </c>
       <c r="X47" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-7.7905645599569553</v>
       </c>
     </row>
@@ -14935,23 +15327,23 @@
         <v>0</v>
       </c>
       <c r="T48" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-14.200484785906454</v>
       </c>
       <c r="U48" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.8046817304370684E-7</v>
       </c>
       <c r="V48" s="22">
-        <f>U48/SUMIF(A:A,A48,U:U)</f>
+        <f t="shared" si="8"/>
         <v>4.1361930515322674E-4</v>
       </c>
       <c r="W48" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.1361930515322674E-4</v>
       </c>
       <c r="X48" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-7.7905645599569553</v>
       </c>
     </row>
@@ -15014,23 +15406,23 @@
         <v>0</v>
       </c>
       <c r="T49" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-15.14881134250904</v>
       </c>
       <c r="U49" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.6360571802287428E-7</v>
       </c>
       <c r="V49" s="22">
-        <f>U49/SUMIF(A:A,A49,U:U)</f>
+        <f t="shared" si="8"/>
         <v>1.6023146745473938E-4</v>
       </c>
       <c r="W49" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.6023146745473938E-4</v>
       </c>
       <c r="X49" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-8.7388911165595413</v>
       </c>
     </row>
@@ -15093,23 +15485,23 @@
         <v>0</v>
       </c>
       <c r="T50" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-15.14881134250904</v>
       </c>
       <c r="U50" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.6360571802287428E-7</v>
       </c>
       <c r="V50" s="24">
-        <f>U50/SUMIF(A:A,A50,U:U)</f>
+        <f t="shared" si="8"/>
         <v>0.99878140448065533</v>
       </c>
       <c r="W50" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.99878140448065533</v>
       </c>
       <c r="X50" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-1.2193386106110198E-3</v>
       </c>
     </row>
@@ -15172,23 +15564,23 @@
         <v>0</v>
       </c>
       <c r="T51" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-23.136441153066734</v>
       </c>
       <c r="U51" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.9530554927975837E-11</v>
       </c>
       <c r="V51" s="22">
-        <f>U51/SUMIF(A:A,A51,U:U)</f>
+        <f t="shared" si="8"/>
         <v>3.3922425532186917E-4</v>
       </c>
       <c r="W51" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.3922425532186917E-4</v>
       </c>
       <c r="X51" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-7.9888491491683054</v>
       </c>
     </row>
@@ -15251,23 +15643,23 @@
         <v>0</v>
       </c>
       <c r="T52" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-22.184019460628335</v>
       </c>
       <c r="U52" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.3206132190589675E-10</v>
       </c>
       <c r="V52" s="22">
-        <f>U52/SUMIF(A:A,A52,U:U)</f>
+        <f t="shared" si="8"/>
         <v>8.7926216000631875E-4</v>
       </c>
       <c r="W52" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.7926216000631875E-4</v>
       </c>
       <c r="X52" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-7.0364274567299052</v>
       </c>
     </row>
@@ -15330,23 +15722,23 @@
         <v>0</v>
       </c>
       <c r="T53" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-31.178556131530591</v>
       </c>
       <c r="U53" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.8795532782154758E-14</v>
       </c>
       <c r="V53" s="22">
-        <f>U53/SUMIF(A:A,A53,U:U)</f>
+        <f t="shared" si="8"/>
         <v>1.0910401675138779E-7</v>
       </c>
       <c r="W53" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.0910401675138779E-7</v>
       </c>
       <c r="X53" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-16.030964127632163</v>
       </c>
     </row>
@@ -15409,23 +15801,23 @@
         <v>0</v>
       </c>
       <c r="T54" s="35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-15.14881134250904</v>
       </c>
       <c r="U54" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.6360571802287428E-7</v>
       </c>
       <c r="V54" s="35">
-        <f>U54/SUMIF(A:A,A54,U:U)</f>
+        <f t="shared" si="8"/>
         <v>0.9973671000731823</v>
       </c>
       <c r="W54" s="35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.9973671000731823</v>
       </c>
       <c r="X54" s="35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-2.6363721037653922E-3</v>
       </c>
     </row>
@@ -15488,23 +15880,23 @@
         <v>1</v>
       </c>
       <c r="T55" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-21.499065755319151</v>
       </c>
       <c r="U55" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.6033540293598718E-10</v>
       </c>
       <c r="V55" s="22">
-        <f>U55/SUMIF(A:A,A55,U:U)</f>
+        <f t="shared" si="8"/>
         <v>1.7417049574298125E-3</v>
       </c>
       <c r="W55" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.7417049574298125E-3</v>
       </c>
       <c r="X55" s="22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-6.3528907849138765</v>
       </c>
     </row>
@@ -15567,23 +15959,23 @@
         <v>0</v>
       </c>
       <c r="T56" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-22.169244562499546</v>
       </c>
       <c r="U56" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.3551545872088013E-10</v>
       </c>
       <c r="V56" s="22">
-        <f>U56/SUMIF(A:A,A56,U:U)</f>
+        <f t="shared" si="8"/>
         <v>8.9108601986572433E-4</v>
       </c>
       <c r="W56" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.9108601986572433E-4</v>
       </c>
       <c r="X56" s="22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-7.0230695920942718</v>
       </c>
     </row>
@@ -15646,23 +16038,23 @@
         <v>0</v>
       </c>
       <c r="T57" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-31.178556131530591</v>
       </c>
       <c r="U57" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.8795532782154758E-14</v>
       </c>
       <c r="V57" s="22">
-        <f>U57/SUMIF(A:A,A57,U:U)</f>
+        <f t="shared" si="8"/>
         <v>1.0894952219324697E-7</v>
       </c>
       <c r="W57" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.0894952219324697E-7</v>
       </c>
       <c r="X57" s="22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-16.032381161125315</v>
       </c>
     </row>
@@ -15697,7 +16089,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{850AC650-7A5B-7B40-A7B3-9A73DB585324}">
   <dimension ref="A1:K11"/>
   <sheetViews>

</xml_diff>

<commit_message>
simple perceptron learning from a pre-defined tableau works now
</commit_message>
<xml_diff>
--- a/Combo/sampleTableaux.xlsx
+++ b/Combo/sampleTableaux.xlsx
@@ -8,99 +8,101 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clairemoore-cantwell/GitHub/GSR_Learning/Combo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB203C02-2D5B-BF4B-8F93-258FCCDB1172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6070CE90-D1E6-D742-8A64-727312B3A911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="2220" windowWidth="28800" windowHeight="17540" xr2:uid="{6D016418-8590-7F42-9768-866F63012115}"/>
+    <workbookView xWindow="9020" yWindow="2480" windowWidth="28780" windowHeight="16580" xr2:uid="{6D016418-8590-7F42-9768-866F63012115}"/>
   </bookViews>
   <sheets>
-    <sheet name="LikelihoodCalcEx" sheetId="7" r:id="rId1"/>
-    <sheet name="GSRTab" sheetId="1" r:id="rId2"/>
-    <sheet name="GSRTab_hidden" sheetId="6" r:id="rId3"/>
-    <sheet name="RSTTab" sheetId="2" r:id="rId4"/>
-    <sheet name="RSTTab_hidden" sheetId="3" r:id="rId5"/>
-    <sheet name="secretCalculator" sheetId="5" r:id="rId6"/>
+    <sheet name="Voicing_example" sheetId="9" r:id="rId1"/>
+    <sheet name="LikelihoodCalcEx" sheetId="7" r:id="rId2"/>
+    <sheet name="GSRTab" sheetId="1" r:id="rId3"/>
+    <sheet name="GSRTab_hidden" sheetId="6" r:id="rId4"/>
+    <sheet name="RSTTab" sheetId="2" r:id="rId5"/>
+    <sheet name="RSTTab_hidden" sheetId="3" r:id="rId6"/>
+    <sheet name="secretCalculator" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">GSRTab!$E$5:$R$5</definedName>
-    <definedName name="solver_adj" localSheetId="3" hidden="1">RSTTab!$E$5:$R$5</definedName>
-    <definedName name="solver_adj" localSheetId="4" hidden="1">RSTTab_hidden!$F$6:$S$6</definedName>
-    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
-    <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">GSRTab!$E$5:$R$5</definedName>
+    <definedName name="solver_adj" localSheetId="4" hidden="1">RSTTab!$E$5:$R$5</definedName>
+    <definedName name="solver_adj" localSheetId="5" hidden="1">RSTTab_hidden!$F$6:$S$6</definedName>
+    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_cvg" localSheetId="5" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_eng" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
-    <definedName name="solver_lin" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_lin" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_itr" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_lin" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_lin" localSheetId="4" hidden="1">2</definedName>
-    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_lin" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
-    <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
+    <definedName name="solver_mip" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
-    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
-    <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
+    <definedName name="solver_mni" localSheetId="5" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
-    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_mrt" localSheetId="5" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_msl" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_neg" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_num" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_nod" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_num" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">GSRTab!$X$9</definedName>
-    <definedName name="solver_opt" localSheetId="3" hidden="1">RSTTab!$X$8</definedName>
-    <definedName name="solver_opt" localSheetId="4" hidden="1">RSTTab_hidden!$Z$11</definedName>
-    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
-    <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
+    <definedName name="solver_num" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">GSRTab!$X$9</definedName>
+    <definedName name="solver_opt" localSheetId="4" hidden="1">RSTTab!$X$8</definedName>
+    <definedName name="solver_opt" localSheetId="5" hidden="1">RSTTab_hidden!$Z$11</definedName>
+    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
-    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_pre" localSheetId="5" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_rbv" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
-    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_rlx" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rsd" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
-    <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
+    <definedName name="solver_sho" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
-    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_ssz" localSheetId="5" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
-    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
-    <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
+    <definedName name="solver_tim" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_tol" localSheetId="5" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_typ" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_ver" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_ver" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="5" hidden="1">2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -533,7 +535,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="126">
   <si>
     <t>petit_ami</t>
   </si>
@@ -861,12 +863,63 @@
   <si>
     <t>Observed</t>
   </si>
+  <si>
+    <t>Objective:</t>
+  </si>
+  <si>
+    <t>*b</t>
+  </si>
+  <si>
+    <t>*d</t>
+  </si>
+  <si>
+    <t>*g</t>
+  </si>
+  <si>
+    <t>*voice</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>*voicelessObs</t>
+  </si>
+  <si>
+    <t>p, d, k inventory:</t>
+  </si>
+  <si>
+    <t>simple p,t,k inventory:</t>
+  </si>
+  <si>
+    <t>p, d, k inventory with higher token freq on d</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -911,8 +964,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -943,8 +1003,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1034,11 +1106,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF002060"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF002060"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1232,6 +1351,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1744,10 +1886,1581 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB456335-C515-B641-92F1-C074391227C4}">
+  <dimension ref="A1:R165"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="9.33203125" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="3"/>
+    <col min="10" max="10" width="5.6640625" customWidth="1"/>
+    <col min="11" max="11" width="3.6640625" style="76" customWidth="1"/>
+    <col min="12" max="12" width="7.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3">
+        <f>(E7-E5)*SQRT(2)/$C$5^2</f>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f>(F7-F5)*SQRT(2)/$C$5^2</f>
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f>(G7-G5)*SQRT(2)/$C$5^2</f>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f>(H7-H5)*SQRT(2)/$C$5^2</f>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f>(I7-I5)*SQRT(2)/$C$5^2</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="88"/>
+      <c r="L4" s="73"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="88"/>
+      <c r="L5" s="73"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3">
+        <f>(E7-E5)^2/2/$C$5</f>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f>(F7-F5)^2/2/$C$5</f>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f>(G7-G5)^2/2/$C$5</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <f>(H7-H5)^2/2/$C$5</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <f>(I7-I5)^2/2/$C$5</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="88"/>
+      <c r="L6" s="73"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="E7" s="86">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="87">
+        <v>0</v>
+      </c>
+      <c r="I7" s="87">
+        <v>0</v>
+      </c>
+      <c r="J7" s="88"/>
+      <c r="L7" s="73"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="74" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="74" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="74" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="94" t="s">
+        <v>110</v>
+      </c>
+      <c r="F8" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="G8" s="74" t="s">
+        <v>112</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="J8" s="89" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="77" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="75" t="s">
+        <v>114</v>
+      </c>
+      <c r="M8" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="N8" s="74">
+        <f>SUMPRODUCT(M9:M14,C9:C14)</f>
+        <v>-5.3752784076841653</v>
+      </c>
+      <c r="O8" s="74">
+        <f>N8-O10</f>
+        <v>-5.3752784076841653</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="78" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="78" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="78">
+        <v>0</v>
+      </c>
+      <c r="D9" s="78">
+        <v>1</v>
+      </c>
+      <c r="E9" s="92">
+        <v>1</v>
+      </c>
+      <c r="F9" s="78">
+        <v>0</v>
+      </c>
+      <c r="G9" s="78">
+        <v>0</v>
+      </c>
+      <c r="H9" s="78">
+        <v>0</v>
+      </c>
+      <c r="I9" s="78">
+        <v>1</v>
+      </c>
+      <c r="J9" s="90">
+        <f t="shared" ref="J9:J14" si="0">-SUMPRODUCT(E9:I9,E$7:I$7)</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="79">
+        <f t="shared" ref="K9:K14" si="1">EXP(J9)</f>
+        <v>1</v>
+      </c>
+      <c r="L9" s="80">
+        <f t="shared" ref="L9:L14" si="2">K9/SUMIF(A:A,A9,K:K)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M9" s="78">
+        <f t="shared" ref="M9:M14" si="3">LN(L9)</f>
+        <v>-1.791759469228055</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="78" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="78" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" s="78">
+        <v>1</v>
+      </c>
+      <c r="D10" s="78">
+        <v>1</v>
+      </c>
+      <c r="E10" s="92">
+        <v>0</v>
+      </c>
+      <c r="F10" s="78">
+        <v>0</v>
+      </c>
+      <c r="G10" s="78">
+        <v>0</v>
+      </c>
+      <c r="H10" s="78">
+        <v>1</v>
+      </c>
+      <c r="I10" s="78">
+        <v>0</v>
+      </c>
+      <c r="J10" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="79">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L10" s="80">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M10" s="78">
+        <f t="shared" si="3"/>
+        <v>-1.791759469228055</v>
+      </c>
+      <c r="N10" s="81" t="s">
+        <v>116</v>
+      </c>
+      <c r="O10" s="78">
+        <f>SUM(E6:I6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="82" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="82">
+        <v>0</v>
+      </c>
+      <c r="D11" s="82">
+        <v>1</v>
+      </c>
+      <c r="E11" s="93">
+        <v>0</v>
+      </c>
+      <c r="F11" s="82">
+        <v>1</v>
+      </c>
+      <c r="G11" s="82">
+        <v>0</v>
+      </c>
+      <c r="H11" s="82">
+        <v>0</v>
+      </c>
+      <c r="I11" s="82">
+        <v>1</v>
+      </c>
+      <c r="J11" s="91">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="83">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L11" s="84">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M11" s="82">
+        <f t="shared" si="3"/>
+        <v>-1.791759469228055</v>
+      </c>
+      <c r="N11" s="85" t="s">
+        <v>118</v>
+      </c>
+      <c r="O11" s="82">
+        <f>SUM(E4:I4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" s="82" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" s="82" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" s="82">
+        <v>1</v>
+      </c>
+      <c r="D12" s="82">
+        <v>1</v>
+      </c>
+      <c r="E12" s="93">
+        <v>0</v>
+      </c>
+      <c r="F12" s="82">
+        <v>0</v>
+      </c>
+      <c r="G12" s="82">
+        <v>0</v>
+      </c>
+      <c r="H12" s="82">
+        <v>1</v>
+      </c>
+      <c r="I12" s="82">
+        <v>0</v>
+      </c>
+      <c r="J12" s="91">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="83">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L12" s="84">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M12" s="82">
+        <f t="shared" si="3"/>
+        <v>-1.791759469228055</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="78" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="78" t="s">
+        <v>120</v>
+      </c>
+      <c r="C13" s="78">
+        <v>0</v>
+      </c>
+      <c r="D13" s="78">
+        <v>1</v>
+      </c>
+      <c r="E13" s="92">
+        <v>0</v>
+      </c>
+      <c r="F13" s="78">
+        <v>0</v>
+      </c>
+      <c r="G13" s="78">
+        <v>1</v>
+      </c>
+      <c r="H13" s="78">
+        <v>0</v>
+      </c>
+      <c r="I13" s="78">
+        <v>1</v>
+      </c>
+      <c r="J13" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="79">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L13" s="80">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M13" s="78">
+        <f t="shared" si="3"/>
+        <v>-1.791759469228055</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="78" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="78" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14" s="78">
+        <v>1</v>
+      </c>
+      <c r="D14" s="78">
+        <v>1</v>
+      </c>
+      <c r="E14" s="92">
+        <v>0</v>
+      </c>
+      <c r="F14" s="78">
+        <v>0</v>
+      </c>
+      <c r="G14" s="78">
+        <v>0</v>
+      </c>
+      <c r="H14" s="78">
+        <v>1</v>
+      </c>
+      <c r="I14" s="78">
+        <v>0</v>
+      </c>
+      <c r="J14" s="90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="79">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L14" s="80">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M14" s="78">
+        <f t="shared" si="3"/>
+        <v>-1.791759469228055</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="3">
+        <f>(E22-E20)*SQRT(2)/$C$20^2</f>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f>(F22-F20)*SQRT(2)/$C$20^2</f>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f>(G22-G20)*SQRT(2)/$C$20^2</f>
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <f>(H22-H20)*SQRT(2)/$C$20^2</f>
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <f>(I22-I20)*SQRT(2)/$C$20^2</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="88"/>
+      <c r="L19" s="73"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>100</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0</v>
+      </c>
+      <c r="I20" s="3">
+        <v>0</v>
+      </c>
+      <c r="J20" s="88"/>
+      <c r="L20" s="73"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="3">
+        <f>(E22-E20)^2/2/$C$20</f>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <f>(F22-F20)^2/2/$C$20</f>
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f>(G22-G20)^2/2/$C$20</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="3">
+        <f>(H22-H20)^2/2/$C$20</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="3">
+        <f>(I22-I20)^2/2/$C$20</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="88"/>
+      <c r="L21" s="73"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="E22" s="86">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0</v>
+      </c>
+      <c r="H22" s="87">
+        <v>0</v>
+      </c>
+      <c r="I22" s="87">
+        <v>0</v>
+      </c>
+      <c r="J22" s="88"/>
+      <c r="L22" s="73"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="74" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="74" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="74" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="94" t="s">
+        <v>110</v>
+      </c>
+      <c r="F23" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="G23" s="74" t="s">
+        <v>112</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="J23" s="89" t="s">
+        <v>9</v>
+      </c>
+      <c r="K23" s="77" t="s">
+        <v>10</v>
+      </c>
+      <c r="L23" s="75" t="s">
+        <v>114</v>
+      </c>
+      <c r="M23" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="N23" s="74">
+        <f>SUMPRODUCT(M24:M29,C24:C29)</f>
+        <v>-5.3752784076841653</v>
+      </c>
+      <c r="O23" s="74">
+        <f>N23-O25</f>
+        <v>-5.3752784076841653</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="78" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="78" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="78">
+        <v>0</v>
+      </c>
+      <c r="D24" s="78">
+        <v>1</v>
+      </c>
+      <c r="E24" s="92">
+        <v>1</v>
+      </c>
+      <c r="F24" s="78">
+        <v>0</v>
+      </c>
+      <c r="G24" s="78">
+        <v>0</v>
+      </c>
+      <c r="H24" s="78">
+        <v>0</v>
+      </c>
+      <c r="I24" s="78">
+        <v>1</v>
+      </c>
+      <c r="J24" s="90">
+        <f t="shared" ref="J24:J29" si="4">-SUMPRODUCT(E24:I24,E$7:I$7)</f>
+        <v>0</v>
+      </c>
+      <c r="K24" s="79">
+        <f t="shared" ref="K24:K29" si="5">EXP(J24)</f>
+        <v>1</v>
+      </c>
+      <c r="L24" s="80">
+        <f t="shared" ref="L24:L29" si="6">K24/SUMIF(A:A,A24,K:K)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M24" s="78">
+        <f t="shared" ref="M24:M29" si="7">LN(L24)</f>
+        <v>-1.791759469228055</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="78" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25" s="78" t="s">
+        <v>114</v>
+      </c>
+      <c r="C25" s="78">
+        <v>1</v>
+      </c>
+      <c r="D25" s="78">
+        <v>1</v>
+      </c>
+      <c r="E25" s="92">
+        <v>0</v>
+      </c>
+      <c r="F25" s="78">
+        <v>0</v>
+      </c>
+      <c r="G25" s="78">
+        <v>0</v>
+      </c>
+      <c r="H25" s="78">
+        <v>1</v>
+      </c>
+      <c r="I25" s="78">
+        <v>0</v>
+      </c>
+      <c r="J25" s="90">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="79">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="L25" s="80">
+        <f t="shared" si="6"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M25" s="78">
+        <f t="shared" si="7"/>
+        <v>-1.791759469228055</v>
+      </c>
+      <c r="N25" s="81" t="s">
+        <v>116</v>
+      </c>
+      <c r="O25" s="78">
+        <f>SUM(E21:I21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" s="82" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" s="82">
+        <v>1</v>
+      </c>
+      <c r="D26" s="82">
+        <v>1</v>
+      </c>
+      <c r="E26" s="93">
+        <v>0</v>
+      </c>
+      <c r="F26" s="82">
+        <v>1</v>
+      </c>
+      <c r="G26" s="82">
+        <v>0</v>
+      </c>
+      <c r="H26" s="82">
+        <v>0</v>
+      </c>
+      <c r="I26" s="82">
+        <v>1</v>
+      </c>
+      <c r="J26" s="91">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K26" s="83">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="L26" s="84">
+        <f t="shared" si="6"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M26" s="82">
+        <f t="shared" si="7"/>
+        <v>-1.791759469228055</v>
+      </c>
+      <c r="N26" s="85" t="s">
+        <v>118</v>
+      </c>
+      <c r="O26" s="82">
+        <f>SUM(E19:I19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" s="82" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="B27" s="82" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" s="82">
+        <v>0</v>
+      </c>
+      <c r="D27" s="82">
+        <v>1</v>
+      </c>
+      <c r="E27" s="93">
+        <v>0</v>
+      </c>
+      <c r="F27" s="82">
+        <v>0</v>
+      </c>
+      <c r="G27" s="82">
+        <v>0</v>
+      </c>
+      <c r="H27" s="82">
+        <v>1</v>
+      </c>
+      <c r="I27" s="82">
+        <v>0</v>
+      </c>
+      <c r="J27" s="91">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="83">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="L27" s="84">
+        <f t="shared" si="6"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M27" s="82">
+        <f t="shared" si="7"/>
+        <v>-1.791759469228055</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="78" t="s">
+        <v>120</v>
+      </c>
+      <c r="B28" s="78" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="78">
+        <v>0</v>
+      </c>
+      <c r="D28" s="78">
+        <v>1</v>
+      </c>
+      <c r="E28" s="92">
+        <v>0</v>
+      </c>
+      <c r="F28" s="78">
+        <v>0</v>
+      </c>
+      <c r="G28" s="78">
+        <v>1</v>
+      </c>
+      <c r="H28" s="78">
+        <v>0</v>
+      </c>
+      <c r="I28" s="78">
+        <v>1</v>
+      </c>
+      <c r="J28" s="90">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K28" s="79">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="L28" s="80">
+        <f t="shared" si="6"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M28" s="78">
+        <f t="shared" si="7"/>
+        <v>-1.791759469228055</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="78" t="s">
+        <v>120</v>
+      </c>
+      <c r="B29" s="78" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="78">
+        <v>1</v>
+      </c>
+      <c r="D29" s="78">
+        <v>1</v>
+      </c>
+      <c r="E29" s="92">
+        <v>0</v>
+      </c>
+      <c r="F29" s="78">
+        <v>0</v>
+      </c>
+      <c r="G29" s="78">
+        <v>0</v>
+      </c>
+      <c r="H29" s="78">
+        <v>1</v>
+      </c>
+      <c r="I29" s="78">
+        <v>0</v>
+      </c>
+      <c r="J29" s="90">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K29" s="79">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="L29" s="80">
+        <f t="shared" si="6"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M29" s="78">
+        <f t="shared" si="7"/>
+        <v>-1.791759469228055</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="3">
+        <f>(E37-E35)*SQRT(2)/$C$35^2</f>
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <f>(F37-F35)*SQRT(2)/$C$35^2</f>
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <f>(G37-G35)*SQRT(2)/$C$35^2</f>
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <f>(H37-H35)*SQRT(2)/$C$35^2</f>
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <f>(I37-I35)*SQRT(2)/$C$35^2</f>
+        <v>0</v>
+      </c>
+      <c r="J34" s="88"/>
+      <c r="L34" s="73"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>100</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35" s="3">
+        <v>0</v>
+      </c>
+      <c r="I35" s="3">
+        <v>0</v>
+      </c>
+      <c r="J35" s="88"/>
+      <c r="L35" s="73"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="3">
+        <f>(E37-E35)^2/2/$C$35</f>
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <f>(F37-F35)^2/2/$C$35</f>
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <f>(G37-G35)^2/2/$C$35</f>
+        <v>0</v>
+      </c>
+      <c r="H36" s="3">
+        <f>(H37-H35)^2/2/$C$35</f>
+        <v>0</v>
+      </c>
+      <c r="I36" s="3">
+        <f>(I37-I35)^2/2/$C$35</f>
+        <v>0</v>
+      </c>
+      <c r="J36" s="88"/>
+      <c r="L36" s="73"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E37" s="86">
+        <v>0</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0</v>
+      </c>
+      <c r="H37" s="87">
+        <v>0</v>
+      </c>
+      <c r="I37" s="87">
+        <v>0</v>
+      </c>
+      <c r="J37" s="88"/>
+      <c r="L37" s="73"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A38" s="74" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="74" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" s="74" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="94" t="s">
+        <v>110</v>
+      </c>
+      <c r="F38" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="G38" s="74" t="s">
+        <v>112</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="J38" s="89" t="s">
+        <v>9</v>
+      </c>
+      <c r="K38" s="77" t="s">
+        <v>10</v>
+      </c>
+      <c r="L38" s="75" t="s">
+        <v>114</v>
+      </c>
+      <c r="M38" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="N38" s="74">
+        <f>SUMPRODUCT(M39:M44,C39:C44)</f>
+        <v>-5.3752784076841653</v>
+      </c>
+      <c r="O38" s="74">
+        <f>N38-O40</f>
+        <v>-5.3752784076841653</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A39" s="78" t="s">
+        <v>115</v>
+      </c>
+      <c r="B39" s="78" t="s">
+        <v>115</v>
+      </c>
+      <c r="C39" s="78">
+        <v>0</v>
+      </c>
+      <c r="D39" s="78">
+        <v>1</v>
+      </c>
+      <c r="E39" s="92">
+        <v>1</v>
+      </c>
+      <c r="F39" s="78">
+        <v>0</v>
+      </c>
+      <c r="G39" s="78">
+        <v>0</v>
+      </c>
+      <c r="H39" s="78">
+        <v>0</v>
+      </c>
+      <c r="I39" s="78">
+        <v>1</v>
+      </c>
+      <c r="J39" s="90">
+        <f t="shared" ref="J39:J44" si="8">-SUMPRODUCT(E39:I39,E$7:I$7)</f>
+        <v>0</v>
+      </c>
+      <c r="K39" s="79">
+        <f t="shared" ref="K39:K44" si="9">EXP(J39)</f>
+        <v>1</v>
+      </c>
+      <c r="L39" s="80">
+        <f t="shared" ref="L39:L44" si="10">K39/SUMIF(A:A,A39,K:K)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M39" s="78">
+        <f t="shared" ref="M39:M44" si="11">LN(L39)</f>
+        <v>-1.791759469228055</v>
+      </c>
+      <c r="N39" s="78"/>
+      <c r="O39" s="78"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A40" s="78" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="78" t="s">
+        <v>114</v>
+      </c>
+      <c r="C40" s="78">
+        <v>1</v>
+      </c>
+      <c r="D40" s="78">
+        <v>1</v>
+      </c>
+      <c r="E40" s="92">
+        <v>0</v>
+      </c>
+      <c r="F40" s="78">
+        <v>0</v>
+      </c>
+      <c r="G40" s="78">
+        <v>0</v>
+      </c>
+      <c r="H40" s="78">
+        <v>1</v>
+      </c>
+      <c r="I40" s="78">
+        <v>0</v>
+      </c>
+      <c r="J40" s="90">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K40" s="79">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="L40" s="80">
+        <f t="shared" si="10"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M40" s="78">
+        <f t="shared" si="11"/>
+        <v>-1.791759469228055</v>
+      </c>
+      <c r="N40" s="81" t="s">
+        <v>116</v>
+      </c>
+      <c r="O40" s="78">
+        <f>SUM(E36:I36)</f>
+        <v>0</v>
+      </c>
+      <c r="P40" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A41" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="B41" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="C41" s="82">
+        <v>1</v>
+      </c>
+      <c r="D41" s="82">
+        <v>100</v>
+      </c>
+      <c r="E41" s="93">
+        <v>0</v>
+      </c>
+      <c r="F41" s="82">
+        <v>1</v>
+      </c>
+      <c r="G41" s="82">
+        <v>0</v>
+      </c>
+      <c r="H41" s="82">
+        <v>0</v>
+      </c>
+      <c r="I41" s="82">
+        <v>1</v>
+      </c>
+      <c r="J41" s="91">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K41" s="83">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="L41" s="84">
+        <f t="shared" si="10"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M41" s="82">
+        <f t="shared" si="11"/>
+        <v>-1.791759469228055</v>
+      </c>
+      <c r="N41" s="85" t="s">
+        <v>118</v>
+      </c>
+      <c r="O41" s="82">
+        <f>SUM(E34:I34)</f>
+        <v>0</v>
+      </c>
+      <c r="P41" s="74">
+        <f>O41-P43</f>
+        <v>-2</v>
+      </c>
+      <c r="Q41" s="74"/>
+      <c r="R41" s="74"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A42" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="B42" s="82" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" s="82">
+        <v>0</v>
+      </c>
+      <c r="D42" s="82">
+        <v>100</v>
+      </c>
+      <c r="E42" s="93">
+        <v>0</v>
+      </c>
+      <c r="F42" s="82">
+        <v>0</v>
+      </c>
+      <c r="G42" s="82">
+        <v>0</v>
+      </c>
+      <c r="H42" s="82">
+        <v>1</v>
+      </c>
+      <c r="I42" s="82">
+        <v>0</v>
+      </c>
+      <c r="J42" s="91">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K42" s="83">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="L42" s="84">
+        <f t="shared" si="10"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M42" s="82">
+        <f t="shared" si="11"/>
+        <v>-1.791759469228055</v>
+      </c>
+      <c r="N42" s="82"/>
+      <c r="O42" s="82"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A43" s="78" t="s">
+        <v>120</v>
+      </c>
+      <c r="B43" s="78" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" s="78">
+        <v>0</v>
+      </c>
+      <c r="D43" s="78">
+        <v>1</v>
+      </c>
+      <c r="E43" s="92">
+        <v>0</v>
+      </c>
+      <c r="F43" s="78">
+        <v>0</v>
+      </c>
+      <c r="G43" s="78">
+        <v>1</v>
+      </c>
+      <c r="H43" s="78">
+        <v>0</v>
+      </c>
+      <c r="I43" s="78">
+        <v>1</v>
+      </c>
+      <c r="J43" s="90">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K43" s="79">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="L43" s="80">
+        <f t="shared" si="10"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M43" s="78">
+        <f t="shared" si="11"/>
+        <v>-1.791759469228055</v>
+      </c>
+      <c r="N43" s="78"/>
+      <c r="O43" s="78"/>
+      <c r="P43">
+        <f>SUM(E39:J39)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A44" s="78" t="s">
+        <v>120</v>
+      </c>
+      <c r="B44" s="78" t="s">
+        <v>121</v>
+      </c>
+      <c r="C44" s="78">
+        <v>1</v>
+      </c>
+      <c r="D44" s="78">
+        <v>1</v>
+      </c>
+      <c r="E44" s="92">
+        <v>0</v>
+      </c>
+      <c r="F44" s="78">
+        <v>0</v>
+      </c>
+      <c r="G44" s="78">
+        <v>0</v>
+      </c>
+      <c r="H44" s="78">
+        <v>1</v>
+      </c>
+      <c r="I44" s="78">
+        <v>0</v>
+      </c>
+      <c r="J44" s="90">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K44" s="79">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="L44" s="80">
+        <f t="shared" si="10"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M44" s="78">
+        <f t="shared" si="11"/>
+        <v>-1.791759469228055</v>
+      </c>
+      <c r="N44" s="78"/>
+      <c r="O44" s="78"/>
+      <c r="P44">
+        <f>SUM(E37:J37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="55" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="56" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="57" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="58" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="59" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="60" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="61" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="62" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="63" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="64" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="65" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="66" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="67" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="68" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="69" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="70" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="71" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="72" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="73" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="74" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="75" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="76" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="77" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="78" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="79" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="80" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="81" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="82" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="83" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="84" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="85" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="86" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="87" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="88" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="89" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="90" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="91" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="92" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="93" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="94" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="95" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="96" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="97" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="98" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="99" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="100" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="101" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="102" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="103" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="104" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="105" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="106" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="107" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="108" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="109" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="110" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="111" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="112" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="113" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="114" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="115" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="116" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="117" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="118" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="119" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="120" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="121" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="122" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="123" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="124" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="125" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="126" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="127" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="128" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="129" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="130" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="131" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K131" s="95"/>
+    </row>
+    <row r="132" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K132" s="95"/>
+    </row>
+    <row r="133" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K133" s="95"/>
+    </row>
+    <row r="134" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K134" s="95"/>
+    </row>
+    <row r="135" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K135" s="95"/>
+    </row>
+    <row r="136" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K136" s="95"/>
+    </row>
+    <row r="137" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K137" s="95"/>
+    </row>
+    <row r="138" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K138" s="95"/>
+    </row>
+    <row r="139" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K139" s="95"/>
+    </row>
+    <row r="140" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K140" s="95"/>
+    </row>
+    <row r="141" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K141" s="95"/>
+    </row>
+    <row r="142" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K142" s="95"/>
+    </row>
+    <row r="143" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K143" s="95"/>
+    </row>
+    <row r="144" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K144" s="95"/>
+    </row>
+    <row r="145" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K145" s="95"/>
+    </row>
+    <row r="146" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K146" s="95"/>
+    </row>
+    <row r="147" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K147" s="95"/>
+    </row>
+    <row r="148" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K148" s="95"/>
+    </row>
+    <row r="149" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K149" s="95"/>
+    </row>
+    <row r="150" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K150" s="95"/>
+    </row>
+    <row r="151" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K151" s="95"/>
+    </row>
+    <row r="152" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K152" s="95"/>
+    </row>
+    <row r="153" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K153" s="95"/>
+    </row>
+    <row r="154" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K154" s="95"/>
+    </row>
+    <row r="155" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K155" s="95"/>
+    </row>
+    <row r="156" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K156" s="95"/>
+    </row>
+    <row r="157" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K157" s="95"/>
+    </row>
+    <row r="158" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K158" s="95"/>
+    </row>
+    <row r="159" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K159" s="95"/>
+    </row>
+    <row r="160" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K160" s="95"/>
+    </row>
+    <row r="161" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K161" s="95"/>
+    </row>
+    <row r="162" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K162" s="95"/>
+    </row>
+    <row r="163" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K163" s="95"/>
+    </row>
+    <row r="164" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K164" s="95"/>
+    </row>
+    <row r="165" spans="11:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K165" s="95"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="J9:J14" formulaRange="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0046436D-BC8C-DF40-9DB5-7AA4E3FA7FF9}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -1917,7 +3630,7 @@
         <v>-3.4</v>
       </c>
       <c r="G7" s="62">
-        <f t="shared" ref="G7:G11" si="0">EXP(F7)</f>
+        <f>EXP(F7)</f>
         <v>3.337326996032608E-2</v>
       </c>
       <c r="H7" s="63">
@@ -1954,15 +3667,15 @@
         <v>-5.9</v>
       </c>
       <c r="G8" s="62">
-        <f t="shared" si="0"/>
+        <f>EXP(F8)</f>
         <v>2.7394448187683684E-3</v>
       </c>
       <c r="H8" s="63">
-        <f t="shared" ref="H8:H11" si="1">G8/SUMIF(A:A,A8,G:G)</f>
+        <f>G8/SUMIF(A:A,A8,G:G)</f>
         <v>2.0088094972752234E-2</v>
       </c>
       <c r="I8" s="62">
-        <f t="shared" ref="I8:I11" si="2">LN(H8)</f>
+        <f>LN(H8)</f>
         <v>-3.9076279293028922</v>
       </c>
       <c r="J8" s="60"/>
@@ -1991,15 +3704,15 @@
         <v>-2.2999999999999998</v>
       </c>
       <c r="G9" s="62">
-        <f t="shared" si="0"/>
+        <f>EXP(F9)</f>
         <v>0.10025884372280375</v>
       </c>
       <c r="H9" s="63">
-        <f t="shared" si="1"/>
+        <f>G9/SUMIF(A:A,A9,G:G)</f>
         <v>0.7351888093396558</v>
       </c>
       <c r="I9" s="62">
-        <f t="shared" si="2"/>
+        <f>LN(H9)</f>
         <v>-0.30762792930289173</v>
       </c>
       <c r="J9" s="60"/>
@@ -2028,15 +3741,15 @@
         <v>-4.8</v>
       </c>
       <c r="G10" s="70">
-        <f t="shared" si="0"/>
+        <f>EXP(F10)</f>
         <v>8.2297470490200302E-3</v>
       </c>
       <c r="H10" s="71">
-        <f t="shared" si="1"/>
+        <f>G10/SUMIF(A:A,A10,G:G)</f>
         <v>2.4127021417669207E-2</v>
       </c>
       <c r="I10" s="70">
-        <f t="shared" si="2"/>
+        <f>LN(H10)</f>
         <v>-3.7244228459337791</v>
       </c>
       <c r="K10" s="68">
@@ -2064,15 +3777,15 @@
         <v>-1.1000000000000001</v>
       </c>
       <c r="G11" s="62">
-        <f t="shared" si="0"/>
+        <f>EXP(F11)</f>
         <v>0.33287108369807955</v>
       </c>
       <c r="H11" s="63">
-        <f t="shared" si="1"/>
+        <f>G11/SUMIF(A:A,A11,G:G)</f>
         <v>0.9758729785823308</v>
       </c>
       <c r="I11" s="62">
-        <f t="shared" si="2"/>
+        <f>LN(H11)</f>
         <v>-2.442284593377916E-2</v>
       </c>
       <c r="J11" s="60"/>
@@ -2085,16 +3798,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{849952CB-BA06-6C44-855B-3B3D98D8050D}">
   <dimension ref="A2:X50"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane xSplit="2540" ySplit="1800" topLeftCell="B4" activePane="bottomRight"/>
-      <selection sqref="A1:XFD1048576"/>
+      <pane xSplit="2540" ySplit="1800" activePane="bottomRight"/>
+      <selection activeCell="A2" sqref="A1:XFD1048576"/>
       <selection pane="topRight" activeCell="H1" sqref="H1:H50"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6:XFD50"/>
-      <selection pane="bottomRight" activeCell="P15" sqref="P15"/>
+      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4788,7 +6501,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{460165A2-3E40-4443-8001-FC6267ACCC55}">
   <dimension ref="A2:Z56"/>
   <sheetViews>
@@ -8181,7 +9894,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EE4A12C-F81F-5344-95C6-9D393BB4DD30}">
   <dimension ref="A1:X50"/>
   <sheetViews>
@@ -11715,7 +13428,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B73D90-E08E-464C-8F42-5EA90A6C7273}">
   <dimension ref="A1:Z57"/>
   <sheetViews>
@@ -11865,15 +13578,15 @@
         <v>100</v>
       </c>
       <c r="G4" s="6">
-        <f t="shared" ref="G4:S4" si="1">$D$3</f>
+        <f>$D$3</f>
         <v>100</v>
       </c>
       <c r="H4" s="6">
-        <f t="shared" si="1"/>
+        <f>$D$3</f>
         <v>100</v>
       </c>
       <c r="I4" s="6">
-        <f t="shared" si="1"/>
+        <f>$D$3</f>
         <v>100</v>
       </c>
       <c r="J4" s="7">
@@ -11904,7 +13617,7 @@
         <v>1000</v>
       </c>
       <c r="S4" s="21">
-        <f t="shared" si="1"/>
+        <f>$D$3</f>
         <v>100</v>
       </c>
     </row>
@@ -11917,55 +13630,55 @@
         <v>4.3750399210047515E-3</v>
       </c>
       <c r="G5" s="6">
-        <f t="shared" ref="G5:S5" si="2">(G6-G3)^2/2/G4</f>
+        <f t="shared" ref="G5:S5" si="1">(G6-G3)^2/2/G4</f>
         <v>3.5778345170836067E-7</v>
       </c>
       <c r="H5" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I5" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.25252566605366517</v>
       </c>
       <c r="J5" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.5160917087066505E-2</v>
       </c>
       <c r="K5" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.12847635900058177</v>
       </c>
       <c r="L5" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>9.2505056877869057E-2</v>
       </c>
       <c r="M5" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>9.4146866196203854E-2</v>
       </c>
       <c r="N5" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O5" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P5" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q5" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.8885524404753731E-2</v>
       </c>
       <c r="R5" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.8794829754849567E-2</v>
       </c>
       <c r="S5" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.0357014834743992</v>
       </c>
     </row>
@@ -12161,7 +13874,7 @@
         <v>4.6033540293598718E-10</v>
       </c>
       <c r="V8" s="24">
-        <f t="shared" ref="V8:V39" si="3">U8/SUMIF(A:A,A8,U:U)</f>
+        <f t="shared" ref="V8:V39" si="2">U8/SUMIF(A:A,A8,U:U)</f>
         <v>2.7960732692348036E-7</v>
       </c>
       <c r="W8" s="24">
@@ -12232,23 +13945,23 @@
         <v>0</v>
       </c>
       <c r="T9" s="55">
-        <f t="shared" ref="T9:T57" si="4">-SUMPRODUCT(F$6:S$6,F9:S9)</f>
+        <f t="shared" ref="T9:T57" si="3">-SUMPRODUCT(F$6:S$6,F9:S9)</f>
         <v>-7.1066963640451837</v>
       </c>
       <c r="U9" s="56">
-        <f t="shared" ref="U9:U57" si="5">EXP(T9)</f>
+        <f t="shared" ref="U9:U57" si="4">EXP(T9)</f>
         <v>8.1959817848556589E-4</v>
       </c>
       <c r="V9" s="55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.49782322709941496</v>
       </c>
       <c r="W9" s="55" t="str">
-        <f t="shared" ref="W9:W57" si="6">IF(C9=C8,"",SUMIF(C:C,C9,V:V))</f>
+        <f t="shared" ref="W9:W57" si="5">IF(C9=C8,"",SUMIF(C:C,C9,V:V))</f>
         <v/>
       </c>
       <c r="X9" s="58" t="str">
-        <f t="shared" ref="X9:X57" si="7">IF(W9="","NA",LN(W9))</f>
+        <f t="shared" ref="X9:X57" si="6">IF(W9="","NA",LN(W9))</f>
         <v>NA</v>
       </c>
     </row>
@@ -12311,23 +14024,23 @@
         <v>0</v>
       </c>
       <c r="T10" s="55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-14.200484785906454</v>
       </c>
       <c r="U10" s="56">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.8046817304370684E-7</v>
       </c>
       <c r="V10" s="55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>4.133157817273347E-4</v>
       </c>
       <c r="W10" s="55" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X10" s="58" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="X10" s="58" t="str">
-        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
     </row>
@@ -12390,23 +14103,23 @@
         <v>0</v>
       </c>
       <c r="T11" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-7.1022475406298931</v>
       </c>
       <c r="U11" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>8.2325254885008302E-4</v>
       </c>
       <c r="V11" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.50004288850867029</v>
       </c>
       <c r="W11" s="22">
+        <f t="shared" si="5"/>
+        <v>0.50004288850867029</v>
+      </c>
+      <c r="X11" s="29">
         <f t="shared" si="6"/>
-        <v>0.50004288850867029</v>
-      </c>
-      <c r="X11" s="29">
-        <f t="shared" si="7"/>
         <v>-0.69306140722124276</v>
       </c>
       <c r="Y11" s="2" t="s">
@@ -12476,23 +14189,23 @@
         <v>0</v>
       </c>
       <c r="T12" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-14.200484785906454</v>
       </c>
       <c r="U12" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.8046817304370684E-7</v>
       </c>
       <c r="V12" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>4.133157817273347E-4</v>
       </c>
       <c r="W12" s="22">
+        <f t="shared" si="5"/>
+        <v>4.133157817273347E-4</v>
+      </c>
+      <c r="X12" s="29">
         <f t="shared" si="6"/>
-        <v>4.133157817273347E-4</v>
-      </c>
-      <c r="X12" s="29">
-        <f t="shared" si="7"/>
         <v>-7.7912986524978036</v>
       </c>
       <c r="Y12" s="2" t="s">
@@ -12562,23 +14275,23 @@
         <v>0</v>
       </c>
       <c r="T13" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-14.200484785906454</v>
       </c>
       <c r="U13" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.8046817304370684E-7</v>
       </c>
       <c r="V13" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>4.133157817273347E-4</v>
       </c>
       <c r="W13" s="22">
+        <f t="shared" si="5"/>
+        <v>4.133157817273347E-4</v>
+      </c>
+      <c r="X13" s="29">
         <f t="shared" si="6"/>
-        <v>4.133157817273347E-4</v>
-      </c>
-      <c r="X13" s="29">
-        <f t="shared" si="7"/>
         <v>-7.7912986524978036</v>
       </c>
     </row>
@@ -12641,23 +14354,23 @@
         <v>0</v>
       </c>
       <c r="T14" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-14.200484785906454</v>
       </c>
       <c r="U14" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.8046817304370684E-7</v>
       </c>
       <c r="V14" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>4.133157817273347E-4</v>
       </c>
       <c r="W14" s="22">
+        <f t="shared" si="5"/>
+        <v>4.133157817273347E-4</v>
+      </c>
+      <c r="X14" s="29">
         <f t="shared" si="6"/>
-        <v>4.133157817273347E-4</v>
-      </c>
-      <c r="X14" s="29">
-        <f t="shared" si="7"/>
         <v>-7.7912986524978036</v>
       </c>
     </row>
@@ -12720,23 +14433,23 @@
         <v>0</v>
       </c>
       <c r="T15" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-15.14881134250904</v>
       </c>
       <c r="U15" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.6360571802287428E-7</v>
       </c>
       <c r="V15" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.6011388589282571E-4</v>
       </c>
       <c r="W15" s="22">
+        <f t="shared" si="5"/>
+        <v>1.6011388589282571E-4</v>
+      </c>
+      <c r="X15" s="29">
         <f t="shared" si="6"/>
-        <v>1.6011388589282571E-4</v>
-      </c>
-      <c r="X15" s="29">
-        <f t="shared" si="7"/>
         <v>-8.7396252091003905</v>
       </c>
     </row>
@@ -12799,23 +14512,23 @@
         <v>0</v>
       </c>
       <c r="T16" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-15.14881134250904</v>
       </c>
       <c r="U16" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.6360571802287428E-7</v>
       </c>
       <c r="V16" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.6011388589282571E-4</v>
       </c>
       <c r="W16" s="22">
+        <f t="shared" si="5"/>
+        <v>1.6011388589282571E-4</v>
+      </c>
+      <c r="X16" s="29">
         <f t="shared" si="6"/>
-        <v>1.6011388589282571E-4</v>
-      </c>
-      <c r="X16" s="29">
-        <f t="shared" si="7"/>
         <v>-8.7396252091003905</v>
       </c>
     </row>
@@ -12878,23 +14591,23 @@
         <v>0</v>
       </c>
       <c r="T17" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-15.14881134250904</v>
       </c>
       <c r="U17" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.6360571802287428E-7</v>
       </c>
       <c r="V17" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.6011388589282571E-4</v>
       </c>
       <c r="W17" s="22">
+        <f t="shared" si="5"/>
+        <v>1.6011388589282571E-4</v>
+      </c>
+      <c r="X17" s="29">
         <f t="shared" si="6"/>
-        <v>1.6011388589282571E-4</v>
-      </c>
-      <c r="X17" s="29">
-        <f t="shared" si="7"/>
         <v>-8.7396252091003905</v>
       </c>
     </row>
@@ -12957,23 +14670,23 @@
         <v>1</v>
       </c>
       <c r="T18" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-21.499065755319151</v>
       </c>
       <c r="U18" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.6033540293598718E-10</v>
       </c>
       <c r="V18" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.6027686299772719E-7</v>
       </c>
       <c r="W18" s="24">
+        <f t="shared" si="5"/>
+        <v>0.99753944610011858</v>
+      </c>
+      <c r="X18" s="28">
         <f t="shared" si="6"/>
-        <v>0.99753944610011858</v>
-      </c>
-      <c r="X18" s="28">
-        <f t="shared" si="7"/>
         <v>-2.4635860374750593E-3</v>
       </c>
     </row>
@@ -13036,23 +14749,23 @@
         <v>0</v>
       </c>
       <c r="T19" s="55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-7.1066963640451837</v>
       </c>
       <c r="U19" s="56">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>8.1959817848556589E-4</v>
       </c>
       <c r="V19" s="55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.99753765066033684</v>
       </c>
       <c r="W19" s="55" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X19" s="58" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="X19" s="58" t="str">
-        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
     </row>
@@ -13115,23 +14828,23 @@
         <v>0</v>
       </c>
       <c r="T20" s="55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-20.708538656754584</v>
       </c>
       <c r="U20" s="56">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.014836159438483E-9</v>
       </c>
       <c r="V20" s="55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.2351629186902247E-6</v>
       </c>
       <c r="W20" s="55" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X20" s="58" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="X20" s="58" t="str">
-        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
     </row>
@@ -13194,23 +14907,23 @@
         <v>0</v>
       </c>
       <c r="T21" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-13.610301411478023</v>
       </c>
       <c r="U21" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.2277818243665275E-6</v>
       </c>
       <c r="V21" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.4943403105960144E-3</v>
       </c>
       <c r="W21" s="22">
+        <f t="shared" si="5"/>
+        <v>1.4943403105960144E-3</v>
+      </c>
+      <c r="X21" s="29">
         <f t="shared" si="6"/>
-        <v>1.4943403105960144E-3</v>
-      </c>
-      <c r="X21" s="29">
-        <f t="shared" si="7"/>
         <v>-6.5060704333403896</v>
       </c>
     </row>
@@ -13273,23 +14986,23 @@
         <v>0</v>
       </c>
       <c r="T22" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-20.708538656754584</v>
       </c>
       <c r="U22" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.014836159438483E-9</v>
       </c>
       <c r="V22" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.2351629186902247E-6</v>
       </c>
       <c r="W22" s="22">
+        <f t="shared" si="5"/>
+        <v>1.2351629186902247E-6</v>
+      </c>
+      <c r="X22" s="29">
         <f t="shared" si="6"/>
-        <v>1.2351629186902247E-6</v>
-      </c>
-      <c r="X22" s="29">
-        <f t="shared" si="7"/>
         <v>-13.60430767861695</v>
       </c>
     </row>
@@ -13352,23 +15065,23 @@
         <v>0</v>
       </c>
       <c r="T23" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-20.708538656754584</v>
       </c>
       <c r="U23" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.014836159438483E-9</v>
       </c>
       <c r="V23" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.2351629186902247E-6</v>
       </c>
       <c r="W23" s="22">
+        <f t="shared" si="5"/>
+        <v>1.2351629186902247E-6</v>
+      </c>
+      <c r="X23" s="29">
         <f t="shared" si="6"/>
-        <v>1.2351629186902247E-6</v>
-      </c>
-      <c r="X23" s="29">
-        <f t="shared" si="7"/>
         <v>-13.60430767861695</v>
       </c>
     </row>
@@ -13431,23 +15144,23 @@
         <v>0</v>
       </c>
       <c r="T24" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-20.708538656754584</v>
       </c>
       <c r="U24" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.014836159438483E-9</v>
       </c>
       <c r="V24" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.2351629186902247E-6</v>
       </c>
       <c r="W24" s="22">
+        <f t="shared" si="5"/>
+        <v>1.2351629186902247E-6</v>
+      </c>
+      <c r="X24" s="29">
         <f t="shared" si="6"/>
-        <v>1.2351629186902247E-6</v>
-      </c>
-      <c r="X24" s="29">
-        <f t="shared" si="7"/>
         <v>-13.60430767861695</v>
       </c>
     </row>
@@ -13510,23 +15223,23 @@
         <v>0</v>
       </c>
       <c r="T25" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-15.14881134250904</v>
       </c>
       <c r="U25" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.6360571802287428E-7</v>
       </c>
       <c r="V25" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3.2083603350980383E-4</v>
       </c>
       <c r="W25" s="22">
+        <f t="shared" si="5"/>
+        <v>3.2083603350980383E-4</v>
+      </c>
+      <c r="X25" s="29">
         <f t="shared" si="6"/>
-        <v>3.2083603350980383E-4</v>
-      </c>
-      <c r="X25" s="29">
-        <f t="shared" si="7"/>
         <v>-8.0445803643714058</v>
       </c>
     </row>
@@ -13589,23 +15302,23 @@
         <v>0</v>
       </c>
       <c r="T26" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-15.14881134250904</v>
       </c>
       <c r="U26" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.6360571802287428E-7</v>
       </c>
       <c r="V26" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3.2083603350980383E-4</v>
       </c>
       <c r="W26" s="22">
+        <f t="shared" si="5"/>
+        <v>3.2083603350980383E-4</v>
+      </c>
+      <c r="X26" s="29">
         <f t="shared" si="6"/>
-        <v>3.2083603350980383E-4</v>
-      </c>
-      <c r="X26" s="29">
-        <f t="shared" si="7"/>
         <v>-8.0445803643714058</v>
       </c>
     </row>
@@ -13668,23 +15381,23 @@
         <v>0</v>
       </c>
       <c r="T27" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-15.14881134250904</v>
       </c>
       <c r="U27" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.6360571802287428E-7</v>
       </c>
       <c r="V27" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3.2083603350980383E-4</v>
       </c>
       <c r="W27" s="22">
+        <f t="shared" si="5"/>
+        <v>3.2083603350980383E-4</v>
+      </c>
+      <c r="X27" s="29">
         <f t="shared" si="6"/>
-        <v>3.2083603350980383E-4</v>
-      </c>
-      <c r="X27" s="29">
-        <f t="shared" si="7"/>
         <v>-8.0445803643714058</v>
       </c>
     </row>
@@ -13747,23 +15460,23 @@
         <v>1</v>
       </c>
       <c r="T28" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-21.499065755319151</v>
       </c>
       <c r="U28" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.6033540293598718E-10</v>
       </c>
       <c r="V28" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.6037199704480108E-7</v>
       </c>
       <c r="W28" s="24">
+        <f t="shared" si="5"/>
+        <v>0.99770868669517265</v>
+      </c>
+      <c r="X28" s="28">
         <f t="shared" si="6"/>
-        <v>0.99770868669517265</v>
-      </c>
-      <c r="X28" s="28">
-        <f t="shared" si="7"/>
         <v>-2.2939423799487589E-3</v>
       </c>
     </row>
@@ -13826,23 +15539,23 @@
         <v>0</v>
       </c>
       <c r="T29" s="55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-7.1066963640451837</v>
       </c>
       <c r="U29" s="56">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>8.1959817848556589E-4</v>
       </c>
       <c r="V29" s="55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.99770703083660917</v>
       </c>
       <c r="W29" s="55" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X29" s="58" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="X29" s="58" t="str">
-        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
     </row>
@@ -13905,23 +15618,23 @@
         <v>0</v>
       </c>
       <c r="T30" s="55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-20.828712702484943</v>
       </c>
       <c r="U30" s="56">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>8.9992228846260469E-10</v>
       </c>
       <c r="V30" s="55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.0954865664352183E-6</v>
       </c>
       <c r="W30" s="55" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X30" s="58" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="X30" s="58" t="str">
-        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
     </row>
@@ -13984,23 +15697,23 @@
         <v>0</v>
       </c>
       <c r="T31" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-13.730475457208383</v>
       </c>
       <c r="U31" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.0887552821610829E-6</v>
       </c>
       <c r="V31" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.3253553123797467E-3</v>
       </c>
       <c r="W31" s="22">
+        <f t="shared" si="5"/>
+        <v>1.3253553123797467E-3</v>
+      </c>
+      <c r="X31" s="29">
         <f t="shared" si="6"/>
-        <v>1.3253553123797467E-3</v>
-      </c>
-      <c r="X31" s="29">
-        <f t="shared" si="7"/>
         <v>-6.6260746952058938</v>
       </c>
     </row>
@@ -14063,23 +15776,23 @@
         <v>0</v>
       </c>
       <c r="T32" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-20.828712702484943</v>
       </c>
       <c r="U32" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>8.9992228846260469E-10</v>
       </c>
       <c r="V32" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.0954865664352183E-6</v>
       </c>
       <c r="W32" s="22">
+        <f t="shared" si="5"/>
+        <v>1.0954865664352183E-6</v>
+      </c>
+      <c r="X32" s="29">
         <f t="shared" si="6"/>
-        <v>1.0954865664352183E-6</v>
-      </c>
-      <c r="X32" s="29">
-        <f t="shared" si="7"/>
         <v>-13.724311940482453</v>
       </c>
     </row>
@@ -14142,23 +15855,23 @@
         <v>0</v>
       </c>
       <c r="T33" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-20.828712702484943</v>
       </c>
       <c r="U33" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>8.9992228846260469E-10</v>
       </c>
       <c r="V33" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.0954865664352183E-6</v>
       </c>
       <c r="W33" s="22">
+        <f t="shared" si="5"/>
+        <v>1.0954865664352183E-6</v>
+      </c>
+      <c r="X33" s="29">
         <f t="shared" si="6"/>
-        <v>1.0954865664352183E-6</v>
-      </c>
-      <c r="X33" s="29">
-        <f t="shared" si="7"/>
         <v>-13.724311940482453</v>
       </c>
     </row>
@@ -14221,23 +15934,23 @@
         <v>0</v>
       </c>
       <c r="T34" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-20.828712702484943</v>
       </c>
       <c r="U34" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>8.9992228846260469E-10</v>
       </c>
       <c r="V34" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.0954865664352183E-6</v>
       </c>
       <c r="W34" s="22">
+        <f t="shared" si="5"/>
+        <v>1.0954865664352183E-6</v>
+      </c>
+      <c r="X34" s="29">
         <f t="shared" si="6"/>
-        <v>1.0954865664352183E-6</v>
-      </c>
-      <c r="X34" s="29">
-        <f t="shared" si="7"/>
         <v>-13.724311940482453</v>
       </c>
     </row>
@@ -14300,23 +16013,23 @@
         <v>0</v>
       </c>
       <c r="T35" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-15.14881134250904</v>
       </c>
       <c r="U35" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.6360571802287428E-7</v>
       </c>
       <c r="V35" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3.2089051091611969E-4</v>
       </c>
       <c r="W35" s="22">
+        <f t="shared" si="5"/>
+        <v>3.2089051091611969E-4</v>
+      </c>
+      <c r="X35" s="29">
         <f t="shared" si="6"/>
-        <v>3.2089051091611969E-4</v>
-      </c>
-      <c r="X35" s="29">
-        <f t="shared" si="7"/>
         <v>-8.0444105805065504</v>
       </c>
     </row>
@@ -14379,23 +16092,23 @@
         <v>0</v>
       </c>
       <c r="T36" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-15.14881134250904</v>
       </c>
       <c r="U36" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.6360571802287428E-7</v>
       </c>
       <c r="V36" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3.2089051091611969E-4</v>
       </c>
       <c r="W36" s="22">
+        <f t="shared" si="5"/>
+        <v>3.2089051091611969E-4</v>
+      </c>
+      <c r="X36" s="29">
         <f t="shared" si="6"/>
-        <v>3.2089051091611969E-4</v>
-      </c>
-      <c r="X36" s="29">
-        <f t="shared" si="7"/>
         <v>-8.0444105805065504</v>
       </c>
     </row>
@@ -14458,23 +16171,23 @@
         <v>0</v>
       </c>
       <c r="T37" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-15.14881134250904</v>
       </c>
       <c r="U37" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.6360571802287428E-7</v>
       </c>
       <c r="V37" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3.2089051091611969E-4</v>
       </c>
       <c r="W37" s="22">
+        <f t="shared" si="5"/>
+        <v>3.2089051091611969E-4</v>
+      </c>
+      <c r="X37" s="29">
         <f t="shared" si="6"/>
-        <v>3.2089051091611969E-4</v>
-      </c>
-      <c r="X37" s="29">
-        <f t="shared" si="7"/>
         <v>-8.0444105805065504</v>
       </c>
     </row>
@@ -14537,23 +16250,23 @@
         <v>0</v>
       </c>
       <c r="T38" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-8.459118768623132E-3</v>
       </c>
       <c r="U38" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.99157655890511187</v>
       </c>
       <c r="V38" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.99670438846830645</v>
       </c>
       <c r="W38" s="24">
+        <f t="shared" si="5"/>
+        <v>0.99670438846830645</v>
+      </c>
+      <c r="X38" s="28">
         <f t="shared" si="6"/>
-        <v>0.99670438846830645</v>
-      </c>
-      <c r="X38" s="28">
-        <f t="shared" si="7"/>
         <v>-3.3010540202191721E-3</v>
       </c>
     </row>
@@ -14616,23 +16329,23 @@
         <v>0</v>
       </c>
       <c r="T39" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-7.1066963640451837</v>
       </c>
       <c r="U39" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>8.1959817848556589E-4</v>
       </c>
       <c r="V39" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8.2383664069187238E-4</v>
       </c>
       <c r="W39" s="22">
+        <f t="shared" si="5"/>
+        <v>8.2383664069187238E-4</v>
+      </c>
+      <c r="X39" s="29">
         <f t="shared" si="6"/>
-        <v>8.2383664069187238E-4</v>
-      </c>
-      <c r="X39" s="29">
-        <f t="shared" si="7"/>
         <v>-7.1015382992967799</v>
       </c>
     </row>
@@ -14695,23 +16408,23 @@
         <v>0</v>
       </c>
       <c r="T40" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-7.1066963640451837</v>
       </c>
       <c r="U40" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>8.1959817848556589E-4</v>
       </c>
       <c r="V40" s="22">
-        <f t="shared" ref="V40:V71" si="8">U40/SUMIF(A:A,A40,U:U)</f>
+        <f t="shared" ref="V40:V57" si="7">U40/SUMIF(A:A,A40,U:U)</f>
         <v>8.2383664069187238E-4</v>
       </c>
       <c r="W40" s="22">
+        <f t="shared" si="5"/>
+        <v>8.2383664069187238E-4</v>
+      </c>
+      <c r="X40" s="29">
         <f t="shared" si="6"/>
-        <v>8.2383664069187238E-4</v>
-      </c>
-      <c r="X40" s="29">
-        <f t="shared" si="7"/>
         <v>-7.1015382992967799</v>
       </c>
     </row>
@@ -14774,23 +16487,23 @@
         <v>0</v>
       </c>
       <c r="T41" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-7.1066963640451837</v>
       </c>
       <c r="U41" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>8.1959817848556589E-4</v>
       </c>
       <c r="V41" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>8.2383664069187238E-4</v>
       </c>
       <c r="W41" s="22">
+        <f t="shared" si="5"/>
+        <v>8.2383664069187238E-4</v>
+      </c>
+      <c r="X41" s="29">
         <f t="shared" si="6"/>
-        <v>8.2383664069187238E-4</v>
-      </c>
-      <c r="X41" s="29">
-        <f t="shared" si="7"/>
         <v>-7.1015382992967799</v>
       </c>
     </row>
@@ -14853,23 +16566,23 @@
         <v>0</v>
       </c>
       <c r="T42" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-7.1066963640451837</v>
       </c>
       <c r="U42" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>8.1959817848556589E-4</v>
       </c>
       <c r="V42" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>8.2383664069187238E-4</v>
       </c>
       <c r="W42" s="22">
+        <f t="shared" si="5"/>
+        <v>8.2383664069187238E-4</v>
+      </c>
+      <c r="X42" s="29">
         <f t="shared" si="6"/>
-        <v>8.2383664069187238E-4</v>
-      </c>
-      <c r="X42" s="29">
-        <f t="shared" si="7"/>
         <v>-7.1015382992967799</v>
       </c>
     </row>
@@ -14932,23 +16645,23 @@
         <v>0</v>
       </c>
       <c r="T43" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-15.14881134250904</v>
       </c>
       <c r="U43" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.6360571802287428E-7</v>
       </c>
       <c r="V43" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2.6496892611988438E-7</v>
       </c>
       <c r="W43" s="22">
+        <f t="shared" si="5"/>
+        <v>2.6496892611988438E-7</v>
+      </c>
+      <c r="X43" s="29">
         <f t="shared" si="6"/>
-        <v>2.6496892611988438E-7</v>
-      </c>
-      <c r="X43" s="29">
-        <f t="shared" si="7"/>
         <v>-15.143653277760636</v>
       </c>
     </row>
@@ -15011,23 +16724,23 @@
         <v>0</v>
       </c>
       <c r="T44" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-7.1022475406298931</v>
       </c>
       <c r="U44" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>8.2325254885008302E-4</v>
       </c>
       <c r="V44" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.50041010103072492</v>
       </c>
       <c r="W44" s="24">
+        <f t="shared" si="5"/>
+        <v>0.50041010103072492</v>
+      </c>
+      <c r="X44" s="28">
         <f t="shared" si="6"/>
-        <v>0.50041010103072492</v>
-      </c>
-      <c r="X44" s="28">
-        <f t="shared" si="7"/>
         <v>-0.6923273146803941</v>
       </c>
     </row>
@@ -15090,23 +16803,23 @@
         <v>0</v>
       </c>
       <c r="T45" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-7.1066963640451837</v>
       </c>
       <c r="U45" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>8.1959817848556589E-4</v>
       </c>
       <c r="V45" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.49818880958636075</v>
       </c>
       <c r="W45" s="22">
+        <f t="shared" si="5"/>
+        <v>0.49818880958636075</v>
+      </c>
+      <c r="X45" s="29">
         <f t="shared" si="6"/>
-        <v>0.49818880958636075</v>
-      </c>
-      <c r="X45" s="29">
-        <f t="shared" si="7"/>
         <v>-0.69677613809568473</v>
       </c>
     </row>
@@ -15169,23 +16882,23 @@
         <v>0</v>
       </c>
       <c r="T46" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-14.200484785906454</v>
       </c>
       <c r="U46" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.8046817304370684E-7</v>
       </c>
       <c r="V46" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>4.1361930515322674E-4</v>
       </c>
       <c r="W46" s="22">
+        <f t="shared" si="5"/>
+        <v>4.1361930515322674E-4</v>
+      </c>
+      <c r="X46" s="29">
         <f t="shared" si="6"/>
-        <v>4.1361930515322674E-4</v>
-      </c>
-      <c r="X46" s="29">
-        <f t="shared" si="7"/>
         <v>-7.7905645599569553</v>
       </c>
     </row>
@@ -15248,23 +16961,23 @@
         <v>0</v>
       </c>
       <c r="T47" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-14.200484785906454</v>
       </c>
       <c r="U47" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.8046817304370684E-7</v>
       </c>
       <c r="V47" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>4.1361930515322674E-4</v>
       </c>
       <c r="W47" s="22">
+        <f t="shared" si="5"/>
+        <v>4.1361930515322674E-4</v>
+      </c>
+      <c r="X47" s="29">
         <f t="shared" si="6"/>
-        <v>4.1361930515322674E-4</v>
-      </c>
-      <c r="X47" s="29">
-        <f t="shared" si="7"/>
         <v>-7.7905645599569553</v>
       </c>
     </row>
@@ -15327,23 +17040,23 @@
         <v>0</v>
       </c>
       <c r="T48" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-14.200484785906454</v>
       </c>
       <c r="U48" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.8046817304370684E-7</v>
       </c>
       <c r="V48" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>4.1361930515322674E-4</v>
       </c>
       <c r="W48" s="22">
+        <f t="shared" si="5"/>
+        <v>4.1361930515322674E-4</v>
+      </c>
+      <c r="X48" s="29">
         <f t="shared" si="6"/>
-        <v>4.1361930515322674E-4</v>
-      </c>
-      <c r="X48" s="29">
-        <f t="shared" si="7"/>
         <v>-7.7905645599569553</v>
       </c>
     </row>
@@ -15406,23 +17119,23 @@
         <v>0</v>
       </c>
       <c r="T49" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-15.14881134250904</v>
       </c>
       <c r="U49" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.6360571802287428E-7</v>
       </c>
       <c r="V49" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1.6023146745473938E-4</v>
       </c>
       <c r="W49" s="22">
+        <f t="shared" si="5"/>
+        <v>1.6023146745473938E-4</v>
+      </c>
+      <c r="X49" s="29">
         <f t="shared" si="6"/>
-        <v>1.6023146745473938E-4</v>
-      </c>
-      <c r="X49" s="29">
-        <f t="shared" si="7"/>
         <v>-8.7388911165595413</v>
       </c>
     </row>
@@ -15485,23 +17198,23 @@
         <v>0</v>
       </c>
       <c r="T50" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-15.14881134250904</v>
       </c>
       <c r="U50" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.6360571802287428E-7</v>
       </c>
       <c r="V50" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.99878140448065533</v>
       </c>
       <c r="W50" s="24">
+        <f t="shared" si="5"/>
+        <v>0.99878140448065533</v>
+      </c>
+      <c r="X50" s="28">
         <f t="shared" si="6"/>
-        <v>0.99878140448065533</v>
-      </c>
-      <c r="X50" s="28">
-        <f t="shared" si="7"/>
         <v>-1.2193386106110198E-3</v>
       </c>
     </row>
@@ -15564,23 +17277,23 @@
         <v>0</v>
       </c>
       <c r="T51" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-23.136441153066734</v>
       </c>
       <c r="U51" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>8.9530554927975837E-11</v>
       </c>
       <c r="V51" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>3.3922425532186917E-4</v>
       </c>
       <c r="W51" s="22">
+        <f t="shared" si="5"/>
+        <v>3.3922425532186917E-4</v>
+      </c>
+      <c r="X51" s="29">
         <f t="shared" si="6"/>
-        <v>3.3922425532186917E-4</v>
-      </c>
-      <c r="X51" s="29">
-        <f t="shared" si="7"/>
         <v>-7.9888491491683054</v>
       </c>
     </row>
@@ -15643,23 +17356,23 @@
         <v>0</v>
       </c>
       <c r="T52" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-22.184019460628335</v>
       </c>
       <c r="U52" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.3206132190589675E-10</v>
       </c>
       <c r="V52" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>8.7926216000631875E-4</v>
       </c>
       <c r="W52" s="22">
+        <f t="shared" si="5"/>
+        <v>8.7926216000631875E-4</v>
+      </c>
+      <c r="X52" s="29">
         <f t="shared" si="6"/>
-        <v>8.7926216000631875E-4</v>
-      </c>
-      <c r="X52" s="29">
-        <f t="shared" si="7"/>
         <v>-7.0364274567299052</v>
       </c>
     </row>
@@ -15722,23 +17435,23 @@
         <v>0</v>
       </c>
       <c r="T53" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-31.178556131530591</v>
       </c>
       <c r="U53" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.8795532782154758E-14</v>
       </c>
       <c r="V53" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1.0910401675138779E-7</v>
       </c>
       <c r="W53" s="22">
+        <f t="shared" si="5"/>
+        <v>1.0910401675138779E-7</v>
+      </c>
+      <c r="X53" s="29">
         <f t="shared" si="6"/>
-        <v>1.0910401675138779E-7</v>
-      </c>
-      <c r="X53" s="29">
-        <f t="shared" si="7"/>
         <v>-16.030964127632163</v>
       </c>
     </row>
@@ -15801,23 +17514,23 @@
         <v>0</v>
       </c>
       <c r="T54" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-15.14881134250904</v>
       </c>
       <c r="U54" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.6360571802287428E-7</v>
       </c>
       <c r="V54" s="35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.9973671000731823</v>
       </c>
       <c r="W54" s="35">
+        <f t="shared" si="5"/>
+        <v>0.9973671000731823</v>
+      </c>
+      <c r="X54" s="35">
         <f t="shared" si="6"/>
-        <v>0.9973671000731823</v>
-      </c>
-      <c r="X54" s="35">
-        <f t="shared" si="7"/>
         <v>-2.6363721037653922E-3</v>
       </c>
     </row>
@@ -15880,23 +17593,23 @@
         <v>1</v>
       </c>
       <c r="T55" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-21.499065755319151</v>
       </c>
       <c r="U55" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.6033540293598718E-10</v>
       </c>
       <c r="V55" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1.7417049574298125E-3</v>
       </c>
       <c r="W55" s="22">
+        <f t="shared" si="5"/>
+        <v>1.7417049574298125E-3</v>
+      </c>
+      <c r="X55" s="22">
         <f t="shared" si="6"/>
-        <v>1.7417049574298125E-3</v>
-      </c>
-      <c r="X55" s="22">
-        <f t="shared" si="7"/>
         <v>-6.3528907849138765</v>
       </c>
     </row>
@@ -15959,23 +17672,23 @@
         <v>0</v>
       </c>
       <c r="T56" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-22.169244562499546</v>
       </c>
       <c r="U56" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.3551545872088013E-10</v>
       </c>
       <c r="V56" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>8.9108601986572433E-4</v>
       </c>
       <c r="W56" s="22">
+        <f t="shared" si="5"/>
+        <v>8.9108601986572433E-4</v>
+      </c>
+      <c r="X56" s="22">
         <f t="shared" si="6"/>
-        <v>8.9108601986572433E-4</v>
-      </c>
-      <c r="X56" s="22">
-        <f t="shared" si="7"/>
         <v>-7.0230695920942718</v>
       </c>
     </row>
@@ -16038,23 +17751,23 @@
         <v>0</v>
       </c>
       <c r="T57" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-31.178556131530591</v>
       </c>
       <c r="U57" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.8795532782154758E-14</v>
       </c>
       <c r="V57" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1.0894952219324697E-7</v>
       </c>
       <c r="W57" s="22">
+        <f t="shared" si="5"/>
+        <v>1.0894952219324697E-7</v>
+      </c>
+      <c r="X57" s="22">
         <f t="shared" si="6"/>
-        <v>1.0894952219324697E-7</v>
-      </c>
-      <c r="X57" s="22">
-        <f t="shared" si="7"/>
         <v>-16.032381161125315</v>
       </c>
     </row>
@@ -16089,12 +17802,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{850AC650-7A5B-7B40-A7B3-9A73DB585324}">
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>